<commit_message>
Updated the Excel Sheet to handle more judges
</commit_message>
<xml_diff>
--- a/Excel Examples/Dance Competition Sheet.xlsx
+++ b/Excel Examples/Dance Competition Sheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/Excel Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9913823E-83B6-524A-A48C-AB73F46C5893}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD060CE-AFFE-0B43-81BF-5DFF83041314}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -156,10 +156,55 @@
     <t>EX: 116</t>
   </si>
   <si>
-    <t>Tied 2</t>
+    <t xml:space="preserve">  #+name: rule-8-example-11 </t>
   </si>
   <si>
-    <t>Tied 4</t>
+    <t xml:space="preserve">  | 81 | 2 | 1 | 2 | 1 | 3 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 82 | 4 | 3 | 1 | 2 | 4 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 83 | 5 | 5 | 5 | 4 | 5 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 84 | 3 | 2 | 3 | 5 | 1 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 85 | 1 | 4 | 4 | 3 | 2 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #+name: rule-8-example-30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 81 | 4 | 2 | 2 | 4 | 2 | 6 | 2 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 82 | 5 | 1 | 6 | 5 | 6 | 2 | 6 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 83 | 3 | 3 | 1 | 1 | 1 | 1 | 1 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 84 | 2 | 5 | 5 | 3 | 4 | 3 | 5 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 85 | 6 | 6 | 4 | 6 | 5 | 4 | 3 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 86 | 1 | 4 | 3 | 2 | 3 | 5 | 2 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 81 | 2 | 4 | 1 | 4 | 1 | 2 | 4 | 3 | 4 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 82 | 4 | 1 | 3 | 3 | 4 | 1 | 1 | 4 | 2 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 83 | 3 | 3 | 4 | 2 | 2 | 4 | 2 | 2 | 3 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 84 | 1 | 2 | 2 | 1 | 3 | 3 | 3 | 1 | 1 |</t>
   </si>
 </sst>
 </file>
@@ -868,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -933,6 +978,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="49" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -940,6 +1007,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,43 +1048,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1094,109 +1143,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1208,6 +1155,12 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1221,17 +1174,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1242,6 +1195,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1255,17 +1215,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1276,6 +1236,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1289,17 +1256,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1310,6 +1277,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1323,126 +1297,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1453,34 +1318,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
+        <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1491,17 +1359,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thick">
+        <right style="thin">
           <color auto="1"/>
         </right>
         <top style="thin">
@@ -1510,17 +1379,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1531,10 +1400,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1550,8 +1420,53 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1922,16 +1837,152 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thick">
           <color auto="1"/>
         </left>
         <right style="thick">
           <color auto="1"/>
         </right>
-        <bottom style="thick">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1951,15 +2002,234 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2485,16 +2755,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3020,6 +3280,174 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -3157,409 +3585,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0"/>
+    </dxf>
+    <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Helvetica"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0"/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3838,7 +3887,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A958EBC6-E5F9-FA41-8059-1514ABF7AAB6}" name="Table5" displayName="Table5" ref="A26:V33" totalsRowShown="0" headerRowDxfId="86" headerRowBorderDxfId="85" tableBorderDxfId="84" headerRowCellStyle="Check Cell">
   <autoFilter ref="A26:V33" xr:uid="{18BC5C1E-6C7F-C542-9C1F-F30AB8500471}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{57D02D44-66F8-094D-A76F-6C1117FE30CE}" name="No. " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{57D02D44-66F8-094D-A76F-6C1117FE30CE}" name="No. " dataDxfId="83"/>
     <tableColumn id="2" xr3:uid="{8573DB78-D3F6-9B45-B90F-232F0946DBFA}" name="A"/>
     <tableColumn id="3" xr3:uid="{C4C572C3-2C00-1645-A12C-65D22A358FB8}" name="B"/>
     <tableColumn id="4" xr3:uid="{4D5F7649-4742-3842-9806-2161D13B3144}" name="C"/>
@@ -3847,49 +3896,49 @@
     <tableColumn id="7" xr3:uid="{AA514D78-B7B6-1743-BAFD-15B51C407E29}" name="F"/>
     <tableColumn id="8" xr3:uid="{EF3B4FBB-0C8D-554E-8B02-F92BC8B72E85}" name="G"/>
     <tableColumn id="9" xr3:uid="{5552FB60-D882-4A47-8164-EC8DDA1384E1}" name="H"/>
-    <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="82">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="82"/>
+    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="9">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="81">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="8">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="80">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="7">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="79">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="6">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="78">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="5">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="77">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="4">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="76">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
+    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="3">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="75">
-      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="2">
+      <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="1">
-      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="0">
-      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="74"/>
-    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="73"/>
+    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="20"/>
+    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" headerRowCellStyle="Check Cell">
   <autoFilter ref="A35:J42" xr:uid="{822117C4-C240-004D-9F32-86F10EF15DB6}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="78">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{91B188C1-5953-B947-9C2F-3BC1268D9E07}" name="A"/>
@@ -3907,10 +3956,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" headerRowCellStyle="Check Cell">
   <autoFilter ref="A44:J51" xr:uid="{FA9CCF3B-D2B7-8745-911A-41DE0BA2D56E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="74">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{560C67EF-0E22-1D49-915D-041AF7EA89CB}" name="A"/>
@@ -3928,10 +3977,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" headerRowCellStyle="Check Cell">
   <autoFilter ref="A53:J60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="61">
+    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="70">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{2D0B4B6B-9866-B847-A7FC-C3BCC560EF8B}" name="A"/>
@@ -3949,141 +3998,141 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67" headerRowCellStyle="Check Cell">
   <autoFilter ref="K35:V42" xr:uid="{26E39BDB-BA98-CD48-AFFD-A777B858DF4A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="57">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="18">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="56">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="17">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="55">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="16">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="54">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="15">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="53">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="14">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="52">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="13">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="51">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="12">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="50">
-      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="11">
+      <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="49">
-      <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="10">
+      <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61" headerRowCellStyle="Check Cell">
   <autoFilter ref="K44:V51" xr:uid="{B523455A-032F-1347-A148-D603C31BEF08}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="60">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="41">
+    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="59">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="40">
+    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="58">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="39">
+    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="57">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="38">
+    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="56">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="37">
+    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="55">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="54">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="53">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="52">
       <calculatedColumnFormula>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46" headerRowCellStyle="Check Cell">
   <autoFilter ref="K53:V60" xr:uid="{6927E80A-15A3-BB47-9D79-AA4675019CC9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="45">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="44">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="43">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="42">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="41">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="40">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="39">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="38">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="19">
+    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="37">
       <calculatedColumnFormula>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30" headerRowCellStyle="Check Cell">
   <autoFilter ref="X26:AF34" xr:uid="{72A9FCD0-51BB-9141-A84C-18D48B93E5C4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="29">
       <calculatedColumnFormula>Table5[[#This Row],[No. ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="24">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4386,12 +4435,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
-  <dimension ref="A2:AF61"/>
+  <dimension ref="A2:AF70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="S28" sqref="S28"/>
+      <selection pane="topRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4406,43 +4455,43 @@
     </row>
     <row r="24" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:32" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="64" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="65"/>
-      <c r="T25" s="65"/>
-      <c r="U25" s="65"/>
-      <c r="V25" s="66"/>
-      <c r="X25" s="67" t="s">
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="75"/>
+      <c r="V25" s="76"/>
+      <c r="X25" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="Y25" s="68"/>
-      <c r="Z25" s="68"/>
-      <c r="AA25" s="68"/>
-      <c r="AB25" s="68"/>
-      <c r="AC25" s="68"/>
-      <c r="AD25" s="68"/>
-      <c r="AE25" s="68"/>
-      <c r="AF25" s="69"/>
+      <c r="Y25" s="83"/>
+      <c r="Z25" s="83"/>
+      <c r="AA25" s="83"/>
+      <c r="AB25" s="83"/>
+      <c r="AC25" s="83"/>
+      <c r="AD25" s="83"/>
+      <c r="AE25" s="83"/>
+      <c r="AF25" s="84"/>
     </row>
     <row r="26" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -4541,89 +4590,89 @@
     </row>
     <row r="27" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B27" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C27" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D27" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E27" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F27" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="19">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
+      <c r="K27" s="54">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
+        <v>2</v>
+      </c>
+      <c r="L27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>4</v>
+      </c>
+      <c r="M27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>5</v>
+      </c>
+      <c r="N27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>5</v>
+      </c>
+      <c r="O27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>5</v>
+      </c>
+      <c r="P27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>5</v>
+      </c>
+      <c r="Q27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>5</v>
+      </c>
+      <c r="R27" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>5</v>
+      </c>
+      <c r="S27" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>9</v>
+      </c>
+      <c r="T27" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>9</v>
+      </c>
+      <c r="U27" s="56"/>
+      <c r="V27" s="57">
         <v>1</v>
-      </c>
-      <c r="O27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>1</v>
-      </c>
-      <c r="P27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>1</v>
-      </c>
-      <c r="Q27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>5</v>
-      </c>
-      <c r="R27" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
-      </c>
-      <c r="S27" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="T27" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="U27" s="31"/>
-      <c r="V27" s="21">
-        <v>7</v>
       </c>
       <c r="X27" s="46">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="Y27" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="45">
-        <f t="shared" ref="Z27:Z33" si="0">V36</f>
-        <v>0</v>
+        <f t="shared" ref="Z27:Z31" si="0">V36</f>
+        <v>3</v>
       </c>
       <c r="AA27" s="45">
-        <f t="shared" ref="AA27:AA33" si="1">V45</f>
+        <f>V45</f>
         <v>0</v>
       </c>
       <c r="AB27" s="45">
-        <f t="shared" ref="AB27:AB33" si="2">V54</f>
+        <f>V54</f>
         <v>0</v>
       </c>
       <c r="AC27" s="45">
@@ -4636,7 +4685,7 @@
       </c>
       <c r="AE27" s="59">
         <f>SUM(Y27:AD27)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AF27" s="52">
         <v>7</v>
@@ -4644,89 +4693,90 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
-        <v>22</v>
+        <f>A27+1</f>
+        <v>82</v>
       </c>
       <c r="B28" s="10">
+        <v>4</v>
+      </c>
+      <c r="C28" s="10">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10">
+        <v>2</v>
+      </c>
+      <c r="E28" s="10">
         <v>1</v>
       </c>
-      <c r="C28" s="10">
-        <v>1</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="10">
-        <v>2</v>
-      </c>
       <c r="F28" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
       <c r="K28" s="54">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
+        <v>1</v>
+      </c>
+      <c r="L28" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>2</v>
+      </c>
+      <c r="M28" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
         <v>3</v>
       </c>
-      <c r="L28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>4</v>
-      </c>
-      <c r="M28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>4</v>
-      </c>
       <c r="N28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>4</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>5</v>
       </c>
       <c r="O28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>5</v>
       </c>
       <c r="P28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
         <v>5</v>
       </c>
       <c r="Q28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
         <v>5</v>
       </c>
       <c r="R28" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
         <v>5</v>
       </c>
       <c r="S28" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>5</v>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>6</v>
       </c>
       <c r="T28" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>5</v>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>14</v>
       </c>
       <c r="U28" s="56"/>
       <c r="V28" s="57">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="X28" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="Y28" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="Z28" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA28" s="45">
-        <f t="shared" si="1"/>
+        <f>V46</f>
         <v>0</v>
       </c>
       <c r="AB28" s="45">
-        <f t="shared" si="2"/>
+        <f>V55</f>
         <v>0</v>
       </c>
       <c r="AC28" s="45">
@@ -4738,8 +4788,8 @@
         <v>0</v>
       </c>
       <c r="AE28" s="59">
-        <f t="shared" ref="AE28:AE33" si="3">SUM(Y28:AD28)</f>
-        <v>1</v>
+        <f t="shared" ref="AE28:AE33" si="1">SUM(Y28:AD28)</f>
+        <v>8.5</v>
       </c>
       <c r="AF28" s="18">
         <v>5</v>
@@ -4747,89 +4797,90 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <v>23</v>
+        <f t="shared" ref="A29:A33" si="2">A28+1</f>
+        <v>83</v>
       </c>
       <c r="B29" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="10">
         <v>5</v>
       </c>
       <c r="D29" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E29" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F29" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="54">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+      <c r="K29" s="19">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
         <v>1</v>
       </c>
-      <c r="N29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>1</v>
-      </c>
-      <c r="O29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>2</v>
-      </c>
-      <c r="P29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
+      <c r="O29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>5</v>
+      </c>
+      <c r="P29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>5</v>
+      </c>
+      <c r="Q29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>5</v>
+      </c>
+      <c r="R29" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>5</v>
+      </c>
+      <c r="S29" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
         <v>4</v>
       </c>
-      <c r="Q29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
+      <c r="U29" s="31"/>
+      <c r="V29" s="21">
         <v>5</v>
-      </c>
-      <c r="R29" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
-      </c>
-      <c r="S29" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="T29" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
-      </c>
-      <c r="U29" s="56"/>
-      <c r="V29" s="57" t="s">
-        <v>44</v>
       </c>
       <c r="X29" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>23</v>
-      </c>
-      <c r="Y29" s="44" t="str">
+        <v>83</v>
+      </c>
+      <c r="Y29" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>Tied 4</v>
+        <v>5</v>
       </c>
       <c r="Z29" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29" s="45">
-        <f t="shared" si="1"/>
+        <f>V47</f>
         <v>0</v>
       </c>
       <c r="AB29" s="45">
-        <f t="shared" si="2"/>
+        <f>V56</f>
         <v>0</v>
       </c>
       <c r="AC29" s="45">
@@ -4841,8 +4892,8 @@
         <v>0</v>
       </c>
       <c r="AE29" s="59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="AF29" s="15">
         <v>2</v>
@@ -4850,10 +4901,11 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>84</v>
       </c>
       <c r="B30" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="10">
         <v>2</v>
@@ -4862,7 +4914,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F30" s="10">
         <v>1</v>
@@ -4872,67 +4924,67 @@
       <c r="I30" s="10"/>
       <c r="J30" s="11"/>
       <c r="K30" s="54">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
         <v>1</v>
       </c>
       <c r="L30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>3</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>2</v>
       </c>
       <c r="M30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
         <v>4</v>
       </c>
       <c r="N30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>4</v>
+      </c>
+      <c r="O30" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>5</v>
       </c>
-      <c r="O30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
+      <c r="P30" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="P30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
+      <c r="Q30" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="Q30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
+      <c r="R30" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="R30" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
-      </c>
       <c r="S30" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>5</v>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>9</v>
       </c>
       <c r="T30" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>8</v>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>9</v>
       </c>
       <c r="U30" s="56"/>
-      <c r="V30" s="57" t="s">
-        <v>43</v>
+      <c r="V30" s="57">
+        <v>2</v>
       </c>
       <c r="X30" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>24</v>
-      </c>
-      <c r="Y30" s="44" t="str">
+        <v>84</v>
+      </c>
+      <c r="Y30" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>Tied 2</v>
+        <v>2</v>
       </c>
       <c r="Z30" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA30" s="45">
-        <f t="shared" si="1"/>
+        <f>V48</f>
         <v>0</v>
       </c>
       <c r="AB30" s="45">
-        <f t="shared" si="2"/>
+        <f>V57</f>
         <v>0</v>
       </c>
       <c r="AC30" s="45">
@@ -4944,8 +4996,8 @@
         <v>0</v>
       </c>
       <c r="AE30" s="59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="AF30" s="15">
         <v>3</v>
@@ -4953,91 +5005,92 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>85</v>
       </c>
       <c r="B31" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D31" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="10">
         <v>3</v>
       </c>
       <c r="F31" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="86">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+      <c r="K31" s="64">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
         <v>1</v>
       </c>
-      <c r="N31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
+      <c r="L31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
         <v>2</v>
       </c>
-      <c r="O31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
-      </c>
-      <c r="P31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
+      <c r="M31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>3</v>
+      </c>
+      <c r="N31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
         <v>5</v>
       </c>
-      <c r="Q31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
+      <c r="O31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>5</v>
       </c>
-      <c r="R31" s="87">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
+      <c r="P31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="S31" s="87">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="87">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
-      </c>
-      <c r="U31" s="88" t="s">
+      <c r="Q31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>5</v>
+      </c>
+      <c r="R31" s="65">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>5</v>
+      </c>
+      <c r="S31" s="65">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>6</v>
+      </c>
+      <c r="T31" s="65">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>14</v>
+      </c>
+      <c r="U31" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="V31" s="89" t="s">
-        <v>44</v>
+      <c r="V31" s="67">
+        <v>3.5</v>
       </c>
       <c r="X31" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>25</v>
-      </c>
-      <c r="Y31" s="44" t="str">
+        <v>85</v>
+      </c>
+      <c r="Y31" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>Tied 4</v>
+        <v>3.5</v>
       </c>
       <c r="Z31" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA31" s="45">
-        <f t="shared" si="1"/>
+        <f>V49</f>
         <v>0</v>
       </c>
       <c r="AB31" s="45">
-        <f t="shared" si="2"/>
+        <f>V58</f>
         <v>0</v>
       </c>
       <c r="AC31" s="45">
@@ -5049,98 +5102,84 @@
         <v>0</v>
       </c>
       <c r="AE31" s="59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.5</v>
       </c>
       <c r="AF31" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
-        <v>26</v>
-      </c>
-      <c r="B32" s="10">
-        <v>4</v>
-      </c>
-      <c r="C32" s="10">
-        <v>3</v>
-      </c>
-      <c r="D32" s="10">
-        <v>2</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10">
-        <v>2</v>
-      </c>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="54">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>1</v>
-      </c>
-      <c r="L32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>3</v>
-      </c>
-      <c r="M32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>4</v>
-      </c>
-      <c r="N32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>5</v>
-      </c>
-      <c r="O32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>5</v>
-      </c>
-      <c r="P32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>5</v>
-      </c>
-      <c r="Q32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>5</v>
-      </c>
-      <c r="R32" s="55">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
-      </c>
-      <c r="S32" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>5</v>
-      </c>
-      <c r="T32" s="55">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>8</v>
-      </c>
-      <c r="U32" s="56"/>
-      <c r="V32" s="57" t="s">
-        <v>43</v>
-      </c>
+      <c r="K32" s="19">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="20">
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="U32" s="31"/>
+      <c r="V32" s="21"/>
       <c r="X32" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>26</v>
-      </c>
-      <c r="Y32" s="44" t="str">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>Tied 2</v>
+        <v>0</v>
       </c>
       <c r="Z32" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>V41</f>
+        <v>2</v>
       </c>
       <c r="AA32" s="45">
-        <f t="shared" si="1"/>
+        <f>V50</f>
         <v>0</v>
       </c>
       <c r="AB32" s="45">
-        <f t="shared" si="2"/>
+        <f>V59</f>
         <v>0</v>
       </c>
       <c r="AC32" s="45">
@@ -5152,98 +5191,84 @@
         <v>0</v>
       </c>
       <c r="AE32" s="59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="AF32" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>27</v>
-      </c>
-      <c r="B33" s="13">
-        <v>3</v>
-      </c>
-      <c r="C33" s="13">
-        <v>4</v>
-      </c>
-      <c r="D33" s="13">
-        <v>6</v>
-      </c>
-      <c r="E33" s="13">
-        <v>5</v>
-      </c>
-      <c r="F33" s="13">
-        <v>5</v>
-      </c>
+      <c r="A33" s="9"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="14"/>
       <c r="K33" s="23">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
         <v>0</v>
       </c>
       <c r="L33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
         <v>0</v>
       </c>
       <c r="M33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>1</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
       </c>
       <c r="N33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>2</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
       </c>
       <c r="O33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
       </c>
       <c r="P33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>5</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
       </c>
       <c r="Q33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>5</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
       </c>
       <c r="R33" s="24">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
+        <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
       </c>
       <c r="S33" s="24">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
         <v>0</v>
       </c>
       <c r="T33" s="24">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
+        <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
       </c>
       <c r="U33" s="33"/>
-      <c r="V33" s="25">
-        <v>6</v>
-      </c>
+      <c r="V33" s="25"/>
       <c r="X33" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="Y33" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="45">
-        <f t="shared" si="0"/>
+        <f>V42</f>
         <v>0</v>
       </c>
       <c r="AA33" s="45">
-        <f t="shared" si="1"/>
+        <f>V51</f>
         <v>0</v>
       </c>
       <c r="AB33" s="45">
-        <f t="shared" si="2"/>
+        <f>V60</f>
         <v>0</v>
       </c>
       <c r="AC33" s="45">
@@ -5255,40 +5280,40 @@
         <v>0</v>
       </c>
       <c r="AE33" s="59">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="AF33" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="64" t="s">
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="65"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="65"/>
-      <c r="O34" s="65"/>
-      <c r="P34" s="65"/>
-      <c r="Q34" s="65"/>
-      <c r="R34" s="65"/>
-      <c r="S34" s="65"/>
-      <c r="T34" s="65"/>
-      <c r="U34" s="65"/>
-      <c r="V34" s="66"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="75"/>
+      <c r="S34" s="75"/>
+      <c r="T34" s="75"/>
+      <c r="U34" s="75"/>
+      <c r="V34" s="76"/>
       <c r="X34" s="48"/>
       <c r="Y34" s="49"/>
       <c r="Z34" s="49"/>
@@ -5371,62 +5396,82 @@
     </row>
     <row r="36" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <f t="shared" ref="A36:A42" si="4">A27</f>
-        <v>21</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
+        <f t="shared" ref="A36:A40" si="3">A27</f>
+        <v>81</v>
+      </c>
+      <c r="B36" s="10">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10">
+        <v>4</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
+        <v>4</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6">
+        <v>2</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4</v>
+      </c>
+      <c r="I36" s="7">
+        <v>3</v>
+      </c>
+      <c r="J36" s="8">
+        <v>4</v>
+      </c>
       <c r="K36" s="19">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
+        <v>2</v>
       </c>
       <c r="L36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>4</v>
       </c>
       <c r="M36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>5</v>
       </c>
       <c r="N36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>9</v>
       </c>
       <c r="O36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>9</v>
       </c>
       <c r="P36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>9</v>
       </c>
       <c r="Q36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>9</v>
       </c>
       <c r="R36" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="55">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>9</v>
+      </c>
+      <c r="S36" s="20">
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>25</v>
       </c>
       <c r="T36" s="20"/>
       <c r="U36" s="31"/>
-      <c r="V36" s="27"/>
+      <c r="V36" s="27">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
-        <f t="shared" si="4"/>
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>82</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -5437,61 +5482,63 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="26">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R37" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S37" s="20">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T37" s="20"/>
-      <c r="U37" s="31"/>
-      <c r="V37" s="27"/>
-      <c r="X37" s="70" t="s">
+      <c r="K37" s="90">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="55">
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="55"/>
+      <c r="U37" s="56"/>
+      <c r="V37" s="91">
+        <v>5</v>
+      </c>
+      <c r="X37" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="Y37" s="71"/>
-      <c r="Z37" s="71"/>
-      <c r="AA37" s="71"/>
-      <c r="AB37" s="71"/>
-      <c r="AC37" s="71"/>
-      <c r="AD37" s="71"/>
-      <c r="AE37" s="71"/>
-      <c r="AF37" s="72"/>
+      <c r="Y37" s="86"/>
+      <c r="Z37" s="86"/>
+      <c r="AA37" s="86"/>
+      <c r="AB37" s="86"/>
+      <c r="AC37" s="86"/>
+      <c r="AD37" s="86"/>
+      <c r="AE37" s="86"/>
+      <c r="AF37" s="87"/>
     </row>
     <row r="38" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <f t="shared" si="4"/>
-        <v>23</v>
+        <f t="shared" si="3"/>
+        <v>83</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -5502,63 +5549,65 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="26">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R38" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="20">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T38" s="20"/>
-      <c r="U38" s="31"/>
-      <c r="V38" s="27"/>
-      <c r="X38" s="84" t="s">
+      <c r="K38" s="90">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="55">
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="55"/>
+      <c r="U38" s="56"/>
+      <c r="V38" s="91">
+        <v>1</v>
+      </c>
+      <c r="X38" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="Y38" s="79"/>
-      <c r="Z38" s="79"/>
-      <c r="AA38" s="79"/>
-      <c r="AB38" s="85"/>
-      <c r="AC38" s="78" t="s">
+      <c r="Y38" s="69"/>
+      <c r="Z38" s="69"/>
+      <c r="AA38" s="69"/>
+      <c r="AB38" s="81"/>
+      <c r="AC38" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="AD38" s="79"/>
-      <c r="AE38" s="79"/>
-      <c r="AF38" s="80"/>
+      <c r="AD38" s="69"/>
+      <c r="AE38" s="69"/>
+      <c r="AF38" s="70"/>
     </row>
     <row r="39" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <f t="shared" si="4"/>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>84</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -5569,45 +5618,47 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="26">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R39" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S39" s="20">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T39" s="20"/>
-      <c r="U39" s="31"/>
-      <c r="V39" s="27"/>
+      <c r="K39" s="90">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="55">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="55">
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="T39" s="55"/>
+      <c r="U39" s="56"/>
+      <c r="V39" s="91">
+        <v>4</v>
+      </c>
       <c r="X39" s="3" t="s">
         <v>27</v>
       </c>
@@ -5637,10 +5688,7 @@
       </c>
     </row>
     <row r="40" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
+      <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -5650,45 +5698,47 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="28">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R40" s="22">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="22">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T40" s="22"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="35"/>
+      <c r="K40" s="92">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="65">
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="65">
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="65"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="93">
+        <v>6</v>
+      </c>
       <c r="X40" s="5" t="s">
         <v>41</v>
       </c>
@@ -5697,27 +5747,27 @@
         <v>0</v>
       </c>
       <c r="Z40" s="10">
-        <f t="shared" ref="Z40:AE45" si="5">SUMIFS(L:L,$A:$A,$X$40)</f>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA40" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB40" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC40" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD40" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE40" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF40" s="8">
@@ -5725,10 +5775,7 @@
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A41" s="9">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
+      <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -5739,73 +5786,75 @@
       <c r="I41" s="10"/>
       <c r="J41" s="11"/>
       <c r="K41" s="26">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
         <v>0</v>
       </c>
       <c r="L41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
         <v>0</v>
       </c>
       <c r="M41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
         <v>0</v>
       </c>
       <c r="N41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
         <v>0</v>
       </c>
       <c r="O41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>0</v>
       </c>
       <c r="P41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
         <v>0</v>
       </c>
       <c r="Q41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
         <v>0</v>
       </c>
       <c r="R41" s="20">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
         <v>0</v>
       </c>
       <c r="S41" s="20">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>0</v>
       </c>
       <c r="T41" s="20"/>
       <c r="U41" s="31"/>
-      <c r="V41" s="27"/>
+      <c r="V41" s="27">
+        <v>2</v>
+      </c>
       <c r="X41" s="9" t="s">
         <v>42</v>
       </c>
       <c r="Y41" s="10">
-        <f t="shared" ref="Y41:Y45" si="6">SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE41" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF41" s="11">
@@ -5813,10 +5862,7 @@
       </c>
     </row>
     <row r="42" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
+      <c r="A42" s="12"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -5827,39 +5873,39 @@
       <c r="I42" s="13"/>
       <c r="J42" s="14"/>
       <c r="K42" s="29">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
         <v>0</v>
       </c>
       <c r="L42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
         <v>0</v>
       </c>
       <c r="M42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
         <v>0</v>
       </c>
       <c r="N42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
         <v>0</v>
       </c>
       <c r="O42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>0</v>
       </c>
       <c r="P42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
         <v>0</v>
       </c>
       <c r="Q42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
         <v>0</v>
       </c>
       <c r="R42" s="30">
-        <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
+        <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
         <v>0</v>
       </c>
       <c r="S42" s="30">
-        <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
+        <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
         <v>0</v>
       </c>
       <c r="T42" s="30"/>
@@ -5867,89 +5913,89 @@
       <c r="V42" s="37"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="10">
-        <f t="shared" si="6"/>
+        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE42" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF42" s="11"/>
     </row>
     <row r="43" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="75" t="s">
+      <c r="A43" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="64" t="s">
+      <c r="B43" s="78"/>
+      <c r="C43" s="78"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="78"/>
+      <c r="J43" s="79"/>
+      <c r="K43" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="65"/>
-      <c r="O43" s="65"/>
-      <c r="P43" s="65"/>
-      <c r="Q43" s="65"/>
-      <c r="R43" s="65"/>
-      <c r="S43" s="65"/>
-      <c r="T43" s="65"/>
-      <c r="U43" s="65"/>
-      <c r="V43" s="66"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="75"/>
+      <c r="P43" s="75"/>
+      <c r="Q43" s="75"/>
+      <c r="R43" s="75"/>
+      <c r="S43" s="75"/>
+      <c r="T43" s="75"/>
+      <c r="U43" s="75"/>
+      <c r="V43" s="76"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="10">
-        <f t="shared" si="6"/>
+        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE43" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF43" s="11"/>
@@ -6023,39 +6069,39 @@
       </c>
       <c r="X44" s="9"/>
       <c r="Y44" s="10">
-        <f t="shared" si="6"/>
+        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE44" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF44" s="11"/>
     </row>
     <row r="45" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <f t="shared" ref="A45:A51" si="7">A27</f>
-        <v>21</v>
+        <f t="shared" ref="A45:A51" si="4">A27</f>
+        <v>81</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -6107,39 +6153,39 @@
       <c r="V45" s="27"/>
       <c r="X45" s="9"/>
       <c r="Y45" s="10">
-        <f t="shared" si="6"/>
+        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AA45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AB45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AC45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AD45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AE45" s="10">
-        <f t="shared" si="5"/>
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="AF45" s="11"/>
     </row>
     <row r="46" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
-        <f t="shared" si="7"/>
-        <v>22</v>
+        <f t="shared" si="4"/>
+        <v>82</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -6201,8 +6247,8 @@
     </row>
     <row r="47" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
-        <f t="shared" si="7"/>
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>83</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -6255,8 +6301,8 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
-        <f t="shared" si="7"/>
-        <v>24</v>
+        <f t="shared" si="4"/>
+        <v>84</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -6309,8 +6355,8 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
-        <f t="shared" si="7"/>
-        <v>25</v>
+        <f t="shared" si="4"/>
+        <v>85</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -6362,10 +6408,7 @@
       <c r="V49" s="35"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A50" s="9">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
+      <c r="A50" s="9"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -6416,10 +6459,7 @@
       <c r="V50" s="27"/>
     </row>
     <row r="51" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
-        <f t="shared" si="7"/>
-        <v>27</v>
-      </c>
+      <c r="A51" s="12"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -6470,32 +6510,32 @@
       <c r="V51" s="37"/>
     </row>
     <row r="52" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="82"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="64" t="s">
+      <c r="B52" s="72"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="72"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L52" s="65"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="65"/>
-      <c r="O52" s="65"/>
-      <c r="P52" s="65"/>
-      <c r="Q52" s="65"/>
-      <c r="R52" s="65"/>
-      <c r="S52" s="65"/>
-      <c r="T52" s="65"/>
-      <c r="U52" s="65"/>
-      <c r="V52" s="66"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="75"/>
+      <c r="N52" s="75"/>
+      <c r="O52" s="75"/>
+      <c r="P52" s="75"/>
+      <c r="Q52" s="75"/>
+      <c r="R52" s="75"/>
+      <c r="S52" s="75"/>
+      <c r="T52" s="75"/>
+      <c r="U52" s="75"/>
+      <c r="V52" s="76"/>
     </row>
     <row r="53" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
@@ -6567,8 +6607,8 @@
     </row>
     <row r="54" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <f t="shared" ref="A54:A60" si="8">A27</f>
-        <v>21</v>
+        <f t="shared" ref="A54:A60" si="5">A27</f>
+        <v>81</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -6621,8 +6661,8 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
-        <f t="shared" si="8"/>
-        <v>22</v>
+        <f t="shared" si="5"/>
+        <v>82</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -6675,8 +6715,8 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
-        <f t="shared" si="8"/>
-        <v>23</v>
+        <f t="shared" si="5"/>
+        <v>83</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -6729,8 +6769,8 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
-        <f t="shared" si="8"/>
-        <v>24</v>
+        <f t="shared" si="5"/>
+        <v>84</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -6783,8 +6823,8 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
-        <f t="shared" si="8"/>
-        <v>25</v>
+        <f t="shared" si="5"/>
+        <v>85</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -6836,10 +6876,7 @@
       <c r="V58" s="35"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A59" s="9">
-        <f t="shared" si="8"/>
-        <v>26</v>
-      </c>
+      <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -6890,10 +6927,7 @@
       <c r="V59" s="27"/>
     </row>
     <row r="60" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12">
-        <f t="shared" si="8"/>
-        <v>27</v>
-      </c>
+      <c r="A60" s="12"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -6944,20 +6978,85 @@
       <c r="V60" s="37"/>
     </row>
     <row r="61" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+      <c r="I64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>50</v>
+      </c>
+      <c r="I65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" t="s">
+        <v>51</v>
+      </c>
+      <c r="I66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" t="s">
+        <v>52</v>
+      </c>
+      <c r="I67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>47</v>
+      </c>
+      <c r="F68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="K25:V25"/>
+    <mergeCell ref="X25:AF25"/>
+    <mergeCell ref="X37:AF37"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="K34:V34"/>
     <mergeCell ref="AC38:AF38"/>
     <mergeCell ref="A52:J52"/>
     <mergeCell ref="K52:V52"/>
     <mergeCell ref="K43:V43"/>
     <mergeCell ref="A43:J43"/>
     <mergeCell ref="X38:AB38"/>
-    <mergeCell ref="K25:V25"/>
-    <mergeCell ref="X25:AF25"/>
-    <mergeCell ref="X37:AF37"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="K34:V34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Only 4 examples left to fix. I just added a check to see if the majorities cascading and then remove them in order and that leaves one bug I think.
</commit_message>
<xml_diff>
--- a/Excel Examples/Dance Competition Sheet.xlsx
+++ b/Excel Examples/Dance Competition Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/Excel Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCEA18D-8E2C-2845-A617-AF14842FE17D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F60397F-1409-E04C-8FC0-8D85582C5D2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18680" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1096,45 +1096,11 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Helvetica"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1166,18 +1132,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1200,6 +1154,71 @@
           <color auto="1"/>
         </left>
         <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -3580,25 +3599,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3965,48 +3965,50 @@
     <tableColumn id="8" xr3:uid="{EF3B4FBB-0C8D-554E-8B02-F92BC8B72E85}" name="G"/>
     <tableColumn id="9" xr3:uid="{5552FB60-D882-4A47-8164-EC8DDA1384E1}" name="H"/>
     <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="84"/>
-    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="18">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="17">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="15">
+    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="16">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="14">
+    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="15">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="13">
+    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="14">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="12">
+    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="13">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="11">
+    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="12">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="10">
+    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="9">
+    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="10">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="8">
+    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="9">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="27"/>
-    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="28"/>
+    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" headerRowCellStyle="Check Cell">
   <autoFilter ref="A35:J42" xr:uid="{822117C4-C240-004D-9F32-86F10EF15DB6}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="2">
+      <calculatedColumnFormula>A27</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" xr3:uid="{91B188C1-5953-B947-9C2F-3BC1268D9E07}" name="A"/>
     <tableColumn id="3" xr3:uid="{ACAD0A10-13F8-9C42-9F09-3D4D95759083}" name="B"/>
     <tableColumn id="4" xr3:uid="{5B77AF9E-BA3D-0A40-8118-53F623648579}" name="C"/>
@@ -4015,7 +4017,7 @@
     <tableColumn id="7" xr3:uid="{D38277F4-96ED-664B-AC61-C274EE8320A0}" name="F"/>
     <tableColumn id="8" xr3:uid="{0EA0170D-5AC0-C14C-8769-DD905DC31CE7}" name="G"/>
     <tableColumn id="9" xr3:uid="{AC046BE1-9636-114E-ADB3-4002117A613F}" name="H"/>
-    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4025,7 +4027,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" headerRowCellStyle="Check Cell">
   <autoFilter ref="A44:J51" xr:uid="{FA9CCF3B-D2B7-8745-911A-41DE0BA2D56E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="1">
+      <calculatedColumnFormula>A27</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" xr3:uid="{560C67EF-0E22-1D49-915D-041AF7EA89CB}" name="A"/>
     <tableColumn id="3" xr3:uid="{E7148EA3-C157-8147-9ED3-7CD2B742719C}" name="B"/>
     <tableColumn id="4" xr3:uid="{6E4594CC-18D1-9140-96A2-A71DC761187A}" name="C"/>
@@ -4034,7 +4038,7 @@
     <tableColumn id="7" xr3:uid="{CE2E0B3B-9098-384F-8DBF-24BB41926824}" name="F"/>
     <tableColumn id="8" xr3:uid="{41FB6D12-D06E-864B-AC53-7B7D2B9ADFEB}" name="G"/>
     <tableColumn id="9" xr3:uid="{A19B9F8B-6EEB-D44D-BE89-44C06042A2AD}" name="H"/>
-    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4044,7 +4048,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78" headerRowCellStyle="Check Cell">
   <autoFilter ref="A53:J60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="0">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{2D0B4B6B-9866-B847-A7FC-C3BCC560EF8B}" name="A"/>
@@ -4062,141 +4066,141 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75" headerRowCellStyle="Check Cell">
   <autoFilter ref="K35:V42" xr:uid="{26E39BDB-BA98-CD48-AFFD-A777B858DF4A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="26">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="25">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="24">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="22">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="21">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="3">
       <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="73"/>
-    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="72"/>
-    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="74"/>
+    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="73"/>
+    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69" headerRowCellStyle="Check Cell">
   <autoFilter ref="K44:V51" xr:uid="{B523455A-032F-1347-A148-D603C31BEF08}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="68">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="66">
+    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="67">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="65">
+    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="66">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="64">
+    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="65">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="63">
+    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="64">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="62">
+    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="63">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="61">
+    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="62">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="60">
+    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="61">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="59">
+    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="60">
       <calculatedColumnFormula>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54" headerRowCellStyle="Check Cell">
   <autoFilter ref="K53:V60" xr:uid="{6927E80A-15A3-BB47-9D79-AA4675019CC9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="53">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="52">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="51">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="50">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="49">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="48">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="47">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="46">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="45">
       <calculatedColumnFormula>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38" headerRowCellStyle="Check Cell">
   <autoFilter ref="X26:AF34" xr:uid="{72A9FCD0-51BB-9141-A84C-18D48B93E5C4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="37">
       <calculatedColumnFormula>Table5[[#This Row],[No. ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="31">
+    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="32">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="31">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4501,10 +4505,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
   <dimension ref="A2:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="S37" sqref="S37"/>
+      <selection pane="topRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4654,22 +4658,22 @@
     </row>
     <row r="27" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B27" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27" s="7">
         <v>2</v>
       </c>
       <c r="E27" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F27" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
@@ -4677,15 +4681,15 @@
       <c r="J27" s="8"/>
       <c r="K27" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L27" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M27" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N27" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
@@ -4709,11 +4713,11 @@
       </c>
       <c r="S27" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T27" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="U27" s="56"/>
       <c r="V27" s="57">
@@ -4721,7 +4725,7 @@
       </c>
       <c r="X27" s="46">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="Y27" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -4757,23 +4761,22 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
-        <f>A27+1</f>
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B28" s="10">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10">
         <v>4</v>
       </c>
-      <c r="C28" s="10">
+      <c r="F28" s="10">
         <v>3</v>
-      </c>
-      <c r="D28" s="10">
-        <v>2</v>
-      </c>
-      <c r="E28" s="10">
-        <v>1</v>
-      </c>
-      <c r="F28" s="10">
-        <v>4</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -4781,7 +4784,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
@@ -4789,7 +4792,7 @@
       </c>
       <c r="M28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
@@ -4813,7 +4816,7 @@
       </c>
       <c r="S28" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="T28" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
@@ -4825,7 +4828,7 @@
       </c>
       <c r="X28" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="Y28" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -4861,23 +4864,22 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <f t="shared" ref="A29:A33" si="2">A28+1</f>
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B29" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D29" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F29" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -4885,19 +4887,19 @@
       <c r="J29" s="11"/>
       <c r="K29" s="19">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
@@ -4917,11 +4919,11 @@
       </c>
       <c r="S29" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T29" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U29" s="31"/>
       <c r="V29" s="21">
@@ -4929,7 +4931,7 @@
       </c>
       <c r="X29" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="Y29" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -4965,23 +4967,22 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
-        <f t="shared" si="2"/>
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="B30" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D30" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30" s="10">
         <v>5</v>
       </c>
       <c r="F30" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -4989,19 +4990,19 @@
       <c r="J30" s="11"/>
       <c r="K30" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
@@ -5021,11 +5022,11 @@
       </c>
       <c r="S30" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="T30" s="55">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U30" s="56"/>
       <c r="V30" s="57">
@@ -5033,7 +5034,7 @@
       </c>
       <c r="X30" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="Y30" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -5069,23 +5070,22 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
-        <f t="shared" si="2"/>
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="B31" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C31" s="10">
+        <v>3</v>
+      </c>
+      <c r="D31" s="10">
+        <v>5</v>
+      </c>
+      <c r="E31" s="10">
+        <v>2</v>
+      </c>
+      <c r="F31" s="10">
         <v>4</v>
-      </c>
-      <c r="D31" s="10">
-        <v>4</v>
-      </c>
-      <c r="E31" s="10">
-        <v>3</v>
-      </c>
-      <c r="F31" s="10">
-        <v>2</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -5093,19 +5093,19 @@
       <c r="J31" s="11"/>
       <c r="K31" s="64">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="65">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31" s="65">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N31" s="65">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O31" s="65">
         <f>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</f>
@@ -5125,11 +5125,11 @@
       </c>
       <c r="S31" s="65">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T31" s="65">
         <f>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="U31" s="66" t="s">
         <v>24</v>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="X31" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="Y31" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -5460,70 +5460,63 @@
     </row>
     <row r="36" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>81</v>
+        <f t="shared" ref="A36:A42" si="2">A27</f>
+        <v>111</v>
       </c>
       <c r="B36" s="10">
+        <v>3</v>
+      </c>
+      <c r="C36" s="10">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10">
         <v>2</v>
       </c>
-      <c r="C36" s="10">
-        <v>1</v>
-      </c>
-      <c r="D36" s="10">
-        <v>6</v>
-      </c>
       <c r="E36" s="10">
+        <v>3</v>
+      </c>
+      <c r="F36" s="10">
         <v>2</v>
       </c>
-      <c r="F36" s="10">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="7">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7">
-        <v>2</v>
-      </c>
-      <c r="J36" s="8">
-        <v>1</v>
-      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="54">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R36" s="55">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S36" s="55">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="T36" s="55"/>
       <c r="U36" s="56"/>
@@ -5533,39 +5526,31 @@
     </row>
     <row r="37" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
-        <f>A36+1</f>
-        <v>82</v>
+        <f t="shared" si="2"/>
+        <v>112</v>
       </c>
       <c r="B37" s="10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C37" s="10">
+        <v>2</v>
+      </c>
+      <c r="D37" s="10">
+        <v>4</v>
+      </c>
+      <c r="E37" s="10">
+        <v>4</v>
+      </c>
+      <c r="F37" s="10">
         <v>3</v>
       </c>
-      <c r="D37" s="10">
-        <v>1</v>
-      </c>
-      <c r="E37" s="10">
-        <v>7</v>
-      </c>
-      <c r="F37" s="10">
-        <v>6</v>
-      </c>
-      <c r="G37" s="10">
-        <v>3</v>
-      </c>
-      <c r="H37" s="10">
-        <v>4</v>
-      </c>
-      <c r="I37" s="10">
-        <v>6</v>
-      </c>
-      <c r="J37" s="11">
-        <v>2</v>
-      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="11"/>
       <c r="K37" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
@@ -5573,7 +5558,7 @@
       </c>
       <c r="M37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
@@ -5585,19 +5570,19 @@
       </c>
       <c r="P37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R37" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S37" s="20">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T37" s="20"/>
       <c r="U37" s="31"/>
@@ -5616,71 +5601,63 @@
     </row>
     <row r="38" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <f t="shared" ref="A38:A42" si="3">A37+1</f>
-        <v>83</v>
+        <f t="shared" si="2"/>
+        <v>113</v>
       </c>
       <c r="B38" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C38" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D38" s="10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E38" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F38" s="10">
-        <v>2</v>
-      </c>
-      <c r="G38" s="10">
-        <v>2</v>
-      </c>
-      <c r="H38" s="10">
-        <v>3</v>
-      </c>
-      <c r="I38" s="10">
-        <v>5</v>
-      </c>
-      <c r="J38" s="11">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="11"/>
       <c r="K38" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Q38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R38" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S38" s="20">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T38" s="20"/>
       <c r="U38" s="31"/>
@@ -5701,71 +5678,63 @@
     </row>
     <row r="39" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <f t="shared" si="3"/>
-        <v>84</v>
+        <f t="shared" si="2"/>
+        <v>114</v>
       </c>
       <c r="B39" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E39" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F39" s="10">
-        <v>35</v>
-      </c>
-      <c r="G39" s="10">
-        <v>6</v>
-      </c>
-      <c r="H39" s="10">
-        <v>7</v>
-      </c>
-      <c r="I39" s="10">
-        <v>1</v>
-      </c>
-      <c r="J39" s="11">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
       <c r="K39" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R39" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S39" s="20">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="T39" s="20"/>
       <c r="U39" s="31"/>
@@ -5800,39 +5769,31 @@
     </row>
     <row r="40" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
-        <f t="shared" si="3"/>
-        <v>85</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="B40" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="10">
         <v>4</v>
       </c>
       <c r="D40" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E40" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F40" s="10">
         <v>4</v>
       </c>
-      <c r="G40" s="10">
-        <v>5</v>
-      </c>
-      <c r="H40" s="10">
-        <v>5</v>
-      </c>
-      <c r="I40" s="10">
-        <v>3</v>
-      </c>
-      <c r="J40" s="11">
-        <v>3</v>
-      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="11"/>
       <c r="K40" s="28">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
@@ -5840,31 +5801,31 @@
       </c>
       <c r="M40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="S40" s="22">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T40" s="22"/>
       <c r="U40" s="32"/>
@@ -5906,71 +5867,53 @@
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="B41" s="10">
-        <v>5</v>
-      </c>
-      <c r="C41" s="10">
-        <v>7</v>
-      </c>
-      <c r="D41" s="10">
-        <v>2</v>
-      </c>
-      <c r="E41" s="10">
-        <v>4</v>
-      </c>
-      <c r="F41" s="10">
-        <v>7</v>
-      </c>
-      <c r="G41" s="10">
-        <v>7</v>
-      </c>
-      <c r="H41" s="10">
-        <v>6</v>
-      </c>
-      <c r="I41" s="10">
-        <v>4</v>
-      </c>
-      <c r="J41" s="11">
-        <v>5</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="11"/>
       <c r="K41" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
         <v>0</v>
       </c>
       <c r="L41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R41" s="20">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S41" s="20">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T41" s="20"/>
       <c r="U41" s="31"/>
@@ -6012,71 +5955,53 @@
     </row>
     <row r="42" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
-        <f t="shared" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="B42" s="13">
-        <v>1</v>
-      </c>
-      <c r="C42" s="13">
-        <v>2</v>
-      </c>
-      <c r="D42" s="13">
-        <v>4</v>
-      </c>
-      <c r="E42" s="13">
-        <v>6</v>
-      </c>
-      <c r="F42" s="13">
-        <v>3</v>
-      </c>
-      <c r="G42" s="13">
-        <v>4</v>
-      </c>
-      <c r="H42" s="13">
-        <v>2</v>
-      </c>
-      <c r="I42" s="13">
-        <v>7</v>
-      </c>
-      <c r="J42" s="14">
-        <v>7</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14"/>
       <c r="K42" s="29">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S42" s="30">
         <f>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T42" s="30"/>
       <c r="U42" s="36"/>
@@ -6270,55 +6195,47 @@
     </row>
     <row r="45" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <f t="shared" ref="A45:A51" si="4">A27</f>
-        <v>81</v>
+        <f t="shared" ref="A45:A51" si="3">A27</f>
+        <v>111</v>
       </c>
       <c r="B45" s="10">
         <v>2</v>
       </c>
       <c r="C45" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D45" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E45" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F45" s="10">
-        <v>1</v>
-      </c>
-      <c r="G45" s="6">
-        <v>1</v>
-      </c>
-      <c r="H45" s="7">
-        <v>1</v>
-      </c>
-      <c r="I45" s="7">
-        <v>2</v>
-      </c>
-      <c r="J45" s="8">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="19">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L45" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M45" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N45" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O45" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P45" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
@@ -6372,59 +6289,51 @@
     </row>
     <row r="46" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
-        <f t="shared" si="4"/>
-        <v>82</v>
+        <f t="shared" si="3"/>
+        <v>112</v>
       </c>
       <c r="B46" s="10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C46" s="10">
+        <v>2</v>
+      </c>
+      <c r="D46" s="10">
         <v>3</v>
       </c>
-      <c r="D46" s="10">
-        <v>1</v>
-      </c>
       <c r="E46" s="10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F46" s="10">
-        <v>6</v>
-      </c>
-      <c r="G46" s="10">
-        <v>3</v>
-      </c>
-      <c r="H46" s="10">
-        <v>4</v>
-      </c>
-      <c r="I46" s="10">
-        <v>6</v>
-      </c>
-      <c r="J46" s="11">
         <v>2</v>
       </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="11"/>
       <c r="K46" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q46" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
@@ -6453,59 +6362,51 @@
     </row>
     <row r="47" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
-        <f t="shared" si="4"/>
-        <v>83</v>
+        <f t="shared" si="3"/>
+        <v>113</v>
       </c>
       <c r="B47" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C47" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D47" s="10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E47" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F47" s="10">
-        <v>2</v>
-      </c>
-      <c r="G47" s="10">
-        <v>2</v>
-      </c>
-      <c r="H47" s="10">
-        <v>3</v>
-      </c>
-      <c r="I47" s="10">
-        <v>5</v>
-      </c>
-      <c r="J47" s="11">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="11"/>
       <c r="K47" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q47" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
@@ -6525,36 +6426,28 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
-        <f t="shared" si="4"/>
-        <v>84</v>
+        <f t="shared" si="3"/>
+        <v>114</v>
       </c>
       <c r="B48" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F48" s="10">
-        <v>35</v>
-      </c>
-      <c r="G48" s="10">
-        <v>6</v>
-      </c>
-      <c r="H48" s="10">
-        <v>7</v>
-      </c>
-      <c r="I48" s="10">
-        <v>1</v>
-      </c>
-      <c r="J48" s="11">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="11"/>
       <c r="K48" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
@@ -6565,27 +6458,27 @@
       </c>
       <c r="M48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R48" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S48" s="20">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -6597,43 +6490,35 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
-        <f t="shared" si="4"/>
-        <v>85</v>
+        <f t="shared" si="3"/>
+        <v>115</v>
       </c>
       <c r="B49" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C49" s="10">
         <v>4</v>
       </c>
       <c r="D49" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49" s="10">
-        <v>4</v>
-      </c>
-      <c r="G49" s="10">
-        <v>5</v>
-      </c>
-      <c r="H49" s="10">
-        <v>5</v>
-      </c>
-      <c r="I49" s="10">
         <v>3</v>
       </c>
-      <c r="J49" s="11">
-        <v>3</v>
-      </c>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="11"/>
       <c r="K49" s="28">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
@@ -6641,7 +6526,7 @@
       </c>
       <c r="N49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
@@ -6669,66 +6554,49 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
-        <v>86</v>
-      </c>
-      <c r="B50" s="10">
-        <v>5</v>
-      </c>
-      <c r="C50" s="10">
-        <v>7</v>
-      </c>
-      <c r="D50" s="10">
-        <v>2</v>
-      </c>
-      <c r="E50" s="10">
-        <v>4</v>
-      </c>
-      <c r="F50" s="10">
-        <v>7</v>
-      </c>
-      <c r="G50" s="10">
-        <v>7</v>
-      </c>
-      <c r="H50" s="10">
-        <v>6</v>
-      </c>
-      <c r="I50" s="10">
-        <v>4</v>
-      </c>
-      <c r="J50" s="11">
-        <v>5</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="11"/>
       <c r="K50" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
       <c r="L50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R50" s="20">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S50" s="20">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -6740,66 +6608,49 @@
     </row>
     <row r="51" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
-        <v>87</v>
-      </c>
-      <c r="B51" s="13">
-        <v>1</v>
-      </c>
-      <c r="C51" s="13">
-        <v>2</v>
-      </c>
-      <c r="D51" s="13">
-        <v>4</v>
-      </c>
-      <c r="E51" s="13">
-        <v>6</v>
-      </c>
-      <c r="F51" s="13">
-        <v>3</v>
-      </c>
-      <c r="G51" s="13">
-        <v>4</v>
-      </c>
-      <c r="H51" s="13">
-        <v>2</v>
-      </c>
-      <c r="I51" s="13">
-        <v>7</v>
-      </c>
-      <c r="J51" s="14">
-        <v>7</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="14"/>
       <c r="K51" s="29">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S51" s="30">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -6907,8 +6758,8 @@
     </row>
     <row r="54" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <f t="shared" ref="A54:A60" si="5">A27</f>
-        <v>81</v>
+        <f t="shared" ref="A54:A60" si="4">A27</f>
+        <v>111</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -6961,8 +6812,8 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
-        <f t="shared" si="5"/>
-        <v>82</v>
+        <f t="shared" si="4"/>
+        <v>112</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -7015,8 +6866,8 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
-        <f t="shared" si="5"/>
-        <v>83</v>
+        <f t="shared" si="4"/>
+        <v>113</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -7069,8 +6920,8 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
-        <f t="shared" si="5"/>
-        <v>84</v>
+        <f t="shared" si="4"/>
+        <v>114</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -7123,8 +6974,8 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
-        <f t="shared" si="5"/>
-        <v>85</v>
+        <f t="shared" si="4"/>
+        <v>115</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -7176,7 +7027,10 @@
       <c r="V58" s="35"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A59" s="9"/>
+      <c r="A59" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -7227,7 +7081,10 @@
       <c r="V59" s="27"/>
     </row>
     <row r="60" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+      <c r="A60" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>

</xml_diff>

<commit_message>
Excel is set up with data needed for example 3
</commit_message>
<xml_diff>
--- a/Excel Examples/Dance Competition Sheet.xlsx
+++ b/Excel Examples/Dance Competition Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/Excel Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F60397F-1409-E04C-8FC0-8D85582C5D2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44FCEE-A6BD-C04B-8457-FF47A0D59E3D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18680" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -150,12 +150,6 @@
     <t>Tie Break SUM #2</t>
   </si>
   <si>
-    <t>EX: 113</t>
-  </si>
-  <si>
-    <t>EX: 116</t>
-  </si>
-  <si>
     <t xml:space="preserve">  #+name: rule-8-example-11 </t>
   </si>
   <si>
@@ -232,6 +226,45 @@
   </si>
   <si>
     <t xml:space="preserve">  #+name: rule-8-example-376</t>
+  </si>
+  <si>
+    <t>Rule 11 Sums</t>
+  </si>
+  <si>
+    <t>Couple</t>
+  </si>
+  <si>
+    <t>Dance # 1</t>
+  </si>
+  <si>
+    <t>Dance # 2</t>
+  </si>
+  <si>
+    <t>Dance # 3</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #+name: rule-8-example-40 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 81 | 5 | 5 | 5 | 5 | 5 | 5 | 5 | 5 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 82 | 1 | 2 | 3 | 1 | 4 | 2 | 3 | 3 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 83 | 2 | 3 | 2 | 3 | 1 | 1 | 1 | 2 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 84 | 3 | 1 | 1 | 2 | 2 | 3 | 2 | 1 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 85 | 4 | 4 | 4 | 4 | 3 | 4 | 4 | 4 |</t>
   </si>
 </sst>
 </file>
@@ -1085,6 +1118,88 @@
   <dxfs count="89">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1249,88 +1364,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3989,10 +4022,10 @@
     <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="10">
+    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="1">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="9">
+    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="0">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="28"/>
@@ -4003,10 +4036,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" headerRowCellStyle="Check Cell">
   <autoFilter ref="A35:J42" xr:uid="{822117C4-C240-004D-9F32-86F10EF15DB6}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="4">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{91B188C1-5953-B947-9C2F-3BC1268D9E07}" name="A"/>
@@ -4017,7 +4050,7 @@
     <tableColumn id="7" xr3:uid="{D38277F4-96ED-664B-AC61-C274EE8320A0}" name="F"/>
     <tableColumn id="8" xr3:uid="{0EA0170D-5AC0-C14C-8769-DD905DC31CE7}" name="G"/>
     <tableColumn id="9" xr3:uid="{AC046BE1-9636-114E-ADB3-4002117A613F}" name="H"/>
-    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4027,7 +4060,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" headerRowCellStyle="Check Cell">
   <autoFilter ref="A44:J51" xr:uid="{FA9CCF3B-D2B7-8745-911A-41DE0BA2D56E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="3">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{560C67EF-0E22-1D49-915D-041AF7EA89CB}" name="A"/>
@@ -4038,7 +4071,7 @@
     <tableColumn id="7" xr3:uid="{CE2E0B3B-9098-384F-8DBF-24BB41926824}" name="F"/>
     <tableColumn id="8" xr3:uid="{41FB6D12-D06E-864B-AC53-7B7D2B9ADFEB}" name="G"/>
     <tableColumn id="9" xr3:uid="{A19B9F8B-6EEB-D44D-BE89-44C06042A2AD}" name="H"/>
-    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4048,7 +4081,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78" headerRowCellStyle="Check Cell">
   <autoFilter ref="A53:J60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="2">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{2D0B4B6B-9866-B847-A7FC-C3BCC560EF8B}" name="A"/>
@@ -4093,7 +4126,7 @@
     <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="5">
       <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="74"/>
@@ -4505,10 +4538,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
   <dimension ref="A2:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="G46" sqref="G46"/>
+      <selection pane="topRight" activeCell="AI38" sqref="AI38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4721,7 +4754,7 @@
       </c>
       <c r="U27" s="56"/>
       <c r="V27" s="57">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="X27" s="46">
         <f>Table5[[#This Row],[No. ]]</f>
@@ -4729,34 +4762,31 @@
       </c>
       <c r="Y27" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Z27" s="45">
-        <f t="shared" ref="Z27:Z31" si="0">V36</f>
-        <v>1</v>
+        <f>V36</f>
+        <v>2</v>
       </c>
       <c r="AA27" s="45">
         <f>V45</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB27" s="45">
         <f>V54</f>
         <v>0</v>
       </c>
-      <c r="AC27" s="45">
-        <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
+      <c r="AC27" s="45"/>
       <c r="AD27" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
       <c r="AE27" s="59">
         <f>SUM(Y27:AD27)</f>
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="AF27" s="52">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
@@ -4824,7 +4854,7 @@
       </c>
       <c r="U28" s="56"/>
       <c r="V28" s="57">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="X28" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
@@ -4832,15 +4862,15 @@
       </c>
       <c r="Y28" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="Z28" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="Z27:Z31" si="0">V37</f>
+        <v>3</v>
       </c>
       <c r="AA28" s="45">
         <f>V46</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB28" s="45">
         <f>V55</f>
@@ -4856,10 +4886,10 @@
       </c>
       <c r="AE28" s="59">
         <f t="shared" ref="AE28:AE33" si="1">SUM(Y28:AD28)</f>
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="AF28" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
@@ -4927,7 +4957,7 @@
       </c>
       <c r="U29" s="31"/>
       <c r="V29" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X29" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
@@ -4935,15 +4965,15 @@
       </c>
       <c r="Y29" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z29" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29" s="45">
         <f>V47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB29" s="45">
         <f>V56</f>
@@ -4959,10 +4989,10 @@
       </c>
       <c r="AE29" s="59">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AF29" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
@@ -5030,7 +5060,7 @@
       </c>
       <c r="U30" s="56"/>
       <c r="V30" s="57">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X30" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
@@ -5038,15 +5068,15 @@
       </c>
       <c r="Y30" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z30" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA30" s="45">
         <f>V48</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB30" s="45">
         <f>V57</f>
@@ -5062,10 +5092,10 @@
       </c>
       <c r="AE30" s="59">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="AF30" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
@@ -5135,7 +5165,7 @@
         <v>24</v>
       </c>
       <c r="V31" s="67">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="X31" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
@@ -5143,15 +5173,15 @@
       </c>
       <c r="Y31" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="Z31" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA31" s="45">
         <f>V49</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB31" s="45">
         <f>V58</f>
@@ -5167,10 +5197,10 @@
       </c>
       <c r="AE31" s="59">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>12</v>
       </c>
       <c r="AF31" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
@@ -5258,9 +5288,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF32" s="18">
-        <v>4</v>
-      </c>
+      <c r="AF32" s="18"/>
     </row>
     <row r="33" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -5347,9 +5375,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF33" s="15">
-        <v>6</v>
-      </c>
+      <c r="AF33" s="15"/>
     </row>
     <row r="34" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="77" t="s">
@@ -5521,7 +5547,7 @@
       <c r="T36" s="55"/>
       <c r="U36" s="56"/>
       <c r="V36" s="90">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
@@ -5586,7 +5612,9 @@
       </c>
       <c r="T37" s="20"/>
       <c r="U37" s="31"/>
-      <c r="V37" s="27"/>
+      <c r="V37" s="27">
+        <v>3</v>
+      </c>
       <c r="X37" s="85" t="s">
         <v>26</v>
       </c>
@@ -5661,7 +5689,9 @@
       </c>
       <c r="T38" s="20"/>
       <c r="U38" s="31"/>
-      <c r="V38" s="27"/>
+      <c r="V38" s="27">
+        <v>1</v>
+      </c>
       <c r="X38" s="80" t="s">
         <v>35</v>
       </c>
@@ -5738,7 +5768,9 @@
       </c>
       <c r="T39" s="20"/>
       <c r="U39" s="31"/>
-      <c r="V39" s="27"/>
+      <c r="V39" s="27">
+        <v>5</v>
+      </c>
       <c r="X39" s="3" t="s">
         <v>27</v>
       </c>
@@ -5829,9 +5861,11 @@
       </c>
       <c r="T40" s="22"/>
       <c r="U40" s="32"/>
-      <c r="V40" s="35"/>
-      <c r="X40" s="5" t="s">
-        <v>41</v>
+      <c r="V40" s="35">
+        <v>4</v>
+      </c>
+      <c r="X40" s="5">
+        <v>111</v>
       </c>
       <c r="Y40" s="10">
         <f>SUMIFS(K:K,$A:$A,$X$40)</f>
@@ -5839,27 +5873,27 @@
       </c>
       <c r="Z40" s="10">
         <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA40" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB40" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC40" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD40" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE40" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF40" s="8">
         <v>5</v>
@@ -5918,36 +5952,36 @@
       <c r="T41" s="20"/>
       <c r="U41" s="31"/>
       <c r="V41" s="27"/>
-      <c r="X41" s="9" t="s">
-        <v>42</v>
+      <c r="X41" s="9">
+        <v>112</v>
       </c>
       <c r="Y41" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f>SUMIFS(K:K,$A:$A,$X$41)</f>
         <v>0</v>
       </c>
       <c r="Z41" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(L:L,$A:$A,$X$41)</f>
+        <v>7</v>
       </c>
       <c r="AA41" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(M:M,$A:$A,$X$41)</f>
+        <v>12</v>
       </c>
       <c r="AB41" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(N:N,$A:$A,$X$41)</f>
+        <v>15</v>
       </c>
       <c r="AC41" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(O:O,$A:$A,$X$41)</f>
+        <v>15</v>
       </c>
       <c r="AD41" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(P:P,$A:$A,$X$41)</f>
+        <v>15</v>
       </c>
       <c r="AE41" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <f>SUMIFS(Q:Q,$A:$A,$X$41)</f>
+        <v>15</v>
       </c>
       <c r="AF41" s="11">
         <v>4</v>
@@ -6013,27 +6047,27 @@
       </c>
       <c r="Z42" s="10">
         <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA42" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB42" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC42" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD42" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE42" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF42" s="11"/>
     </row>
@@ -6071,27 +6105,27 @@
       </c>
       <c r="Z43" s="10">
         <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA43" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB43" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC43" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD43" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE43" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF43" s="11"/>
     </row>
@@ -6169,27 +6203,27 @@
       </c>
       <c r="Z44" s="10">
         <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA44" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB44" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC44" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD44" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE44" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF44" s="11"/>
     </row>
@@ -6255,7 +6289,9 @@
       </c>
       <c r="T45" s="20"/>
       <c r="U45" s="31"/>
-      <c r="V45" s="27"/>
+      <c r="V45" s="27">
+        <v>3</v>
+      </c>
       <c r="X45" s="9"/>
       <c r="Y45" s="10">
         <f>SUMIFS(K:K,$A:$A,$X$40)</f>
@@ -6263,27 +6299,27 @@
       </c>
       <c r="Z45" s="10">
         <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA45" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB45" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC45" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD45" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AE45" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AF45" s="11"/>
     </row>
@@ -6349,7 +6385,9 @@
       </c>
       <c r="T46" s="20"/>
       <c r="U46" s="31"/>
-      <c r="V46" s="27"/>
+      <c r="V46" s="27">
+        <v>2</v>
+      </c>
       <c r="X46" s="12"/>
       <c r="Y46" s="13"/>
       <c r="Z46" s="13"/>
@@ -6360,7 +6398,7 @@
       <c r="AE46" s="14"/>
       <c r="AF46" s="14"/>
     </row>
-    <row r="47" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -6422,9 +6460,11 @@
       </c>
       <c r="T47" s="20"/>
       <c r="U47" s="31"/>
-      <c r="V47" s="27"/>
+      <c r="V47" s="27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -6486,9 +6526,22 @@
       </c>
       <c r="T48" s="20"/>
       <c r="U48" s="31"/>
-      <c r="V48" s="27"/>
+      <c r="V48" s="27">
+        <v>5</v>
+      </c>
+      <c r="X48" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y48" s="86"/>
+      <c r="Z48" s="86"/>
+      <c r="AA48" s="86"/>
+      <c r="AB48" s="86"/>
+      <c r="AC48" s="86"/>
+      <c r="AD48" s="86"/>
+      <c r="AE48" s="86"/>
+      <c r="AF48" s="87"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -6550,9 +6603,24 @@
       </c>
       <c r="T49" s="22"/>
       <c r="U49" s="32"/>
-      <c r="V49" s="35"/>
+      <c r="V49" s="35">
+        <v>4</v>
+      </c>
+      <c r="X49" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y49" s="69"/>
+      <c r="Z49" s="69"/>
+      <c r="AA49" s="69"/>
+      <c r="AB49" s="81"/>
+      <c r="AC49" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD49" s="69"/>
+      <c r="AE49" s="69"/>
+      <c r="AF49" s="70"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6605,8 +6673,35 @@
       <c r="T50" s="20"/>
       <c r="U50" s="31"/>
       <c r="V50" s="27"/>
+      <c r="X50" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>111</v>
+      </c>
+      <c r="Z50" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>111</v>
+      </c>
+      <c r="AB50" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>111</v>
+      </c>
+      <c r="AD50" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE50" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF50" s="53" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="51" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6659,8 +6754,42 @@
       <c r="T51" s="30"/>
       <c r="U51" s="36"/>
       <c r="V51" s="37"/>
+      <c r="X51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y51" s="10">
+        <f>SUMIF(B27:F27, "&lt;=3")</f>
+        <v>10</v>
+      </c>
+      <c r="Z51" s="10">
+        <f>SUMIF(B28:F28, "&lt;=3")</f>
+        <v>10</v>
+      </c>
+      <c r="AA51" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
+        <v>12</v>
+      </c>
+      <c r="AB51" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AC51" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AD51" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AE51" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AF51" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="52" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="71" t="s">
         <v>34</v>
       </c>
@@ -6687,8 +6816,42 @@
       <c r="T52" s="75"/>
       <c r="U52" s="75"/>
       <c r="V52" s="76"/>
+      <c r="X52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y52" s="10">
+        <f>SUMIF(B36:F36, "&lt;=3")</f>
+        <v>13</v>
+      </c>
+      <c r="Z52" s="10">
+        <f>SUMIF(B37:F37, "&lt;=3")</f>
+        <v>7</v>
+      </c>
+      <c r="AA52" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$41)</f>
+        <v>12</v>
+      </c>
+      <c r="AB52" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$41)</f>
+        <v>15</v>
+      </c>
+      <c r="AC52" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$41)</f>
+        <v>15</v>
+      </c>
+      <c r="AD52" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$41)</f>
+        <v>15</v>
+      </c>
+      <c r="AE52" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$41)</f>
+        <v>15</v>
+      </c>
+      <c r="AF52" s="11">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>0</v>
       </c>
@@ -6755,8 +6918,40 @@
       <c r="V53" s="39" t="s">
         <v>19</v>
       </c>
+      <c r="X53" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y53" s="10">
+        <f>SUMIF(B45:F45, "&lt;=3")</f>
+        <v>7</v>
+      </c>
+      <c r="Z53" s="10">
+        <f>SUMIF(B46:F46, "&lt;=3")</f>
+        <v>12</v>
+      </c>
+      <c r="AA53" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
+        <v>12</v>
+      </c>
+      <c r="AB53" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AC53" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AD53" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AE53" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AF53" s="11"/>
     </row>
-    <row r="54" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <f t="shared" ref="A54:A60" si="4">A27</f>
         <v>111</v>
@@ -6809,8 +7004,32 @@
       <c r="T54" s="20"/>
       <c r="U54" s="31"/>
       <c r="V54" s="27"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="10"/>
+      <c r="Z54" s="10"/>
+      <c r="AA54" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
+        <v>12</v>
+      </c>
+      <c r="AB54" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AC54" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AD54" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AE54" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AF54" s="11"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <f t="shared" si="4"/>
         <v>112</v>
@@ -6863,8 +7082,40 @@
       <c r="T55" s="20"/>
       <c r="U55" s="31"/>
       <c r="V55" s="27"/>
+      <c r="X55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y55" s="10">
+        <f>SUM(Y51:Y53)</f>
+        <v>30</v>
+      </c>
+      <c r="Z55" s="10">
+        <f>SUM(Z51:Z53)</f>
+        <v>29</v>
+      </c>
+      <c r="AA55" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
+        <v>12</v>
+      </c>
+      <c r="AB55" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AC55" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AD55" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AE55" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AF55" s="11"/>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <f t="shared" si="4"/>
         <v>113</v>
@@ -6917,8 +7168,32 @@
       <c r="T56" s="20"/>
       <c r="U56" s="31"/>
       <c r="V56" s="27"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="10"/>
+      <c r="Z56" s="10"/>
+      <c r="AA56" s="10">
+        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
+        <v>12</v>
+      </c>
+      <c r="AB56" s="10">
+        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AC56" s="10">
+        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AD56" s="10">
+        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AE56" s="10">
+        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
+        <v>15</v>
+      </c>
+      <c r="AF56" s="11"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <f t="shared" si="4"/>
         <v>114</v>
@@ -6971,8 +7246,17 @@
       <c r="T57" s="20"/>
       <c r="U57" s="31"/>
       <c r="V57" s="27"/>
+      <c r="X57" s="12"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="13"/>
+      <c r="AA57" s="13"/>
+      <c r="AB57" s="13"/>
+      <c r="AC57" s="13"/>
+      <c r="AD57" s="13"/>
+      <c r="AE57" s="14"/>
+      <c r="AF57" s="14"/>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <f t="shared" si="4"/>
         <v>115</v>
@@ -7026,7 +7310,7 @@
       <c r="U58" s="32"/>
       <c r="V58" s="35"/>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7080,7 +7364,7 @@
       <c r="U59" s="31"/>
       <c r="V59" s="27"/>
     </row>
-    <row r="60" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7134,117 +7418,135 @@
       <c r="U60" s="36"/>
       <c r="V60" s="37"/>
     </row>
-    <row r="61" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F64" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I67" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G72" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G73" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G74" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="G75" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G76" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G77" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
     <mergeCell ref="K25:V25"/>
     <mergeCell ref="X25:AF25"/>
     <mergeCell ref="X37:AF37"/>
@@ -7257,6 +7559,9 @@
     <mergeCell ref="K43:V43"/>
     <mergeCell ref="A43:J43"/>
     <mergeCell ref="X38:AB38"/>
+    <mergeCell ref="X48:AF48"/>
+    <mergeCell ref="X49:AB49"/>
+    <mergeCell ref="AC49:AF49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fixed a bug when a quadruple tie where it could be broken by the sum values
</commit_message>
<xml_diff>
--- a/Excel Examples/Dance Competition Sheet.xlsx
+++ b/Excel Examples/Dance Competition Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/Excel Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44FCEE-A6BD-C04B-8457-FF47A0D59E3D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031FF52E-E853-3A41-8175-111A1E00EF8C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="89">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -265,6 +265,33 @@
   </si>
   <si>
     <t xml:space="preserve">  | 85 | 4 | 4 | 4 | 4 | 3 | 4 | 4 | 4 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #+name: mixed-rules-example-60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 21 | 2 | 4 | 6 | 6 | 1 | 3 | 2 | 3 | 5 | 5 | 5 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 22 | 4 | 1 | 5 | 1 | 2 | 4 | 3 | 4 | 1 | 1 | 4 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 23 | 3 | 3 | 4 | 4 | 4 | 6 | 5 | 5 | 2 | 3 | 6 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 24 | 1 | 6 | 1 | 3 | 5 | 5 | 6 | 1 | 6 | 2 | 3 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 25 | 5 | 5 | 3 | 2 | 6 | 1 | 1 | 2 | 4 | 4 | 1 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | 26 | 6 | 2 | 2 | 5 | 3 | 2 | 4 | 6 | 3 | 6 | 2 |</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -973,7 +1000,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1051,33 +1078,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1102,13 +1102,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1116,584 +1148,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="89">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color rgb="FF3F3F3F"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color rgb="FF3F3F3F"/>
-        </left>
-        <right style="double">
-          <color rgb="FF3F3F3F"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2021,80 +1475,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2414,6 +1794,205 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -2939,6 +2518,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3464,16 +3053,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3482,6 +3061,181 @@
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3495,31 +3249,27 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thick">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3533,7 +3283,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -3549,17 +3299,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3570,10 +3320,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -3589,30 +3340,17 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3623,66 +3361,360 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color rgb="FF3F3F3F"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color rgb="FF3F3F3F"/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
         </left>
-        <right style="double">
-          <color rgb="FF3F3F3F"/>
+        <right style="thin">
+          <color auto="1"/>
         </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color rgb="FF3F3F3F"/>
+        <top style="thin">
+          <color auto="1"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color rgb="FF3F3F3F"/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
         </left>
-        <right style="double">
-          <color rgb="FF3F3F3F"/>
+        <right style="thin">
+          <color auto="1"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3998,48 +4030,48 @@
     <tableColumn id="8" xr3:uid="{EF3B4FBB-0C8D-554E-8B02-F92BC8B72E85}" name="G"/>
     <tableColumn id="9" xr3:uid="{5552FB60-D882-4A47-8164-EC8DDA1384E1}" name="H"/>
     <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="84"/>
-    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="83">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="17">
+    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="82">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="16">
+    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="81">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="15">
+    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="80">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="14">
+    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="13">
+    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="78">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="12">
+    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="77">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="11">
+    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="76">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="1">
+    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="75">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="0">
+    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="74">
       <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="28"/>
-    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="73"/>
+    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" headerRowCellStyle="Check Cell">
   <autoFilter ref="A35:J42" xr:uid="{822117C4-C240-004D-9F32-86F10EF15DB6}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="68">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{91B188C1-5953-B947-9C2F-3BC1268D9E07}" name="A"/>
@@ -4050,17 +4082,17 @@
     <tableColumn id="7" xr3:uid="{D38277F4-96ED-664B-AC61-C274EE8320A0}" name="F"/>
     <tableColumn id="8" xr3:uid="{0EA0170D-5AC0-C14C-8769-DD905DC31CE7}" name="G"/>
     <tableColumn id="9" xr3:uid="{AC046BE1-9636-114E-ADB3-4002117A613F}" name="H"/>
-    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{786F3152-0A2A-244B-8A11-B6772B4E2F0E}" name="J" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" headerRowCellStyle="Check Cell">
   <autoFilter ref="A44:J51" xr:uid="{FA9CCF3B-D2B7-8745-911A-41DE0BA2D56E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="63">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{560C67EF-0E22-1D49-915D-041AF7EA89CB}" name="A"/>
@@ -4071,17 +4103,17 @@
     <tableColumn id="7" xr3:uid="{CE2E0B3B-9098-384F-8DBF-24BB41926824}" name="F"/>
     <tableColumn id="8" xr3:uid="{41FB6D12-D06E-864B-AC53-7B7D2B9ADFEB}" name="G"/>
     <tableColumn id="9" xr3:uid="{A19B9F8B-6EEB-D44D-BE89-44C06042A2AD}" name="H"/>
-    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{35194706-BC46-3143-BDF2-5A35036D5200}" name="J" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78" headerRowCellStyle="Check Cell">
-  <autoFilter ref="A53:J60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:L60" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" headerRowCellStyle="Check Cell">
+  <autoFilter ref="A53:L60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="58">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{2D0B4B6B-9866-B847-A7FC-C3BCC560EF8B}" name="A"/>
@@ -4091,149 +4123,151 @@
     <tableColumn id="6" xr3:uid="{731E8778-E29D-B54F-B511-7622B0969955}" name="E"/>
     <tableColumn id="7" xr3:uid="{12E1CD14-3DD2-9C45-81E5-E400A761C3F7}" name="F"/>
     <tableColumn id="8" xr3:uid="{5C472CAF-9A5E-0D40-B886-750396201A31}" name="G"/>
-    <tableColumn id="9" xr3:uid="{26BBD2D1-D95B-0E47-87A1-86E02FE7C392}" name="H"/>
-    <tableColumn id="10" xr3:uid="{43E8327B-F813-A148-B492-BC24E81499CE}" name="J"/>
+    <tableColumn id="13" xr3:uid="{4727ED90-A3E9-5D4E-B5B5-304588331AA8}" name="H"/>
+    <tableColumn id="12" xr3:uid="{B28043B4-9F43-0D47-AE05-E9BB8FD08302}" name="I"/>
+    <tableColumn id="9" xr3:uid="{26BBD2D1-D95B-0E47-87A1-86E02FE7C392}" name="J"/>
+    <tableColumn id="10" xr3:uid="{43E8327B-F813-A148-B492-BC24E81499CE}" name="K"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55" headerRowCellStyle="Check Cell">
   <autoFilter ref="K35:V42" xr:uid="{26E39BDB-BA98-CD48-AFFD-A777B858DF4A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="54">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="53">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="52">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="51">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="50">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="49">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="48">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="47">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[J]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="46">
       <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[J]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="74"/>
-    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40" headerRowCellStyle="Check Cell">
   <autoFilter ref="K44:V51" xr:uid="{B523455A-032F-1347-A148-D603C31BEF08}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="68">
+    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="39">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="38">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="66">
+    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="37">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="65">
+    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="36">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="64">
+    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="35">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="63">
+    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="34">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="62">
+    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="33">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="61">
+    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="32">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="60">
+    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="31">
       <calculatedColumnFormula>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="59"/>
-    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="58"/>
-    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54" headerRowCellStyle="Check Cell">
-  <autoFilter ref="K53:V60" xr:uid="{6927E80A-15A3-BB47-9D79-AA4675019CC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="M53:X60" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25" headerRowCellStyle="Check Cell">
+  <autoFilter ref="M53:X60" xr:uid="{6927E80A-15A3-BB47-9D79-AA4675019CC9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="53">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="7">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="52">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="6">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="51">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="5">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="50">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="4">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="49">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="3">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="48">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="2">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="47">
-      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="46">
+    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="24">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="45">
-      <calculatedColumnFormula>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="0">
+      <calculatedColumnFormula>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17" headerRowCellStyle="Check Cell">
   <autoFilter ref="X26:AF34" xr:uid="{72A9FCD0-51BB-9141-A84C-18D48B93E5C4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="16">
       <calculatedColumnFormula>Table5[[#This Row],[No. ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="10">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4536,12 +4570,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
-  <dimension ref="A2:AF79"/>
+  <dimension ref="A2:AH79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="AI38" sqref="AI38"/>
+      <selection pane="topRight" activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4556,43 +4590,43 @@
     </row>
     <row r="24" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:32" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="85" t="s">
+      <c r="A25" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="89"/>
-      <c r="K25" s="74" t="s">
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="75"/>
-      <c r="S25" s="75"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="75"/>
-      <c r="V25" s="76"/>
-      <c r="X25" s="82" t="s">
+      <c r="L25" s="81"/>
+      <c r="M25" s="81"/>
+      <c r="N25" s="81"/>
+      <c r="O25" s="81"/>
+      <c r="P25" s="81"/>
+      <c r="Q25" s="81"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
+      <c r="V25" s="82"/>
+      <c r="X25" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="Y25" s="83"/>
-      <c r="Z25" s="83"/>
-      <c r="AA25" s="83"/>
-      <c r="AB25" s="83"/>
-      <c r="AC25" s="83"/>
-      <c r="AD25" s="83"/>
-      <c r="AE25" s="83"/>
-      <c r="AF25" s="84"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="74"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="74"/>
+      <c r="AF25" s="75"/>
     </row>
     <row r="26" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -4691,7 +4725,7 @@
     </row>
     <row r="27" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B27" s="6">
         <v>3</v>
@@ -4758,7 +4792,7 @@
       </c>
       <c r="X27" s="46">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="Y27" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -4769,12 +4803,12 @@
         <v>2</v>
       </c>
       <c r="AA27" s="45">
-        <f>V45</f>
+        <f t="shared" ref="AA27:AA33" si="0">V45</f>
         <v>3</v>
       </c>
       <c r="AB27" s="45">
-        <f>V54</f>
-        <v>0</v>
+        <f t="shared" ref="AB27:AB33" si="1">X54</f>
+        <v>6</v>
       </c>
       <c r="AC27" s="45"/>
       <c r="AD27" s="58">
@@ -4783,7 +4817,7 @@
       </c>
       <c r="AE27" s="59">
         <f>SUM(Y27:AD27)</f>
-        <v>7.5</v>
+        <v>13.5</v>
       </c>
       <c r="AF27" s="52">
         <v>3</v>
@@ -4791,7 +4825,8 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
-        <v>112</v>
+        <f>A27+1</f>
+        <v>22</v>
       </c>
       <c r="B28" s="10">
         <v>2</v>
@@ -4858,23 +4893,23 @@
       </c>
       <c r="X28" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="Y28" s="44">
         <f>Table5[[#This Row],[Result]]</f>
         <v>2.5</v>
       </c>
       <c r="Z28" s="45">
-        <f t="shared" ref="Z27:Z31" si="0">V37</f>
+        <f t="shared" ref="Z28:Z31" si="2">V37</f>
         <v>3</v>
       </c>
       <c r="AA28" s="45">
-        <f>V46</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AB28" s="45">
-        <f>V55</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AC28" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
@@ -4885,8 +4920,8 @@
         <v>0</v>
       </c>
       <c r="AE28" s="59">
-        <f t="shared" ref="AE28:AE33" si="1">SUM(Y28:AD28)</f>
-        <v>7.5</v>
+        <f t="shared" ref="AE28:AE33" si="3">SUM(Y28:AD28)</f>
+        <v>8.5</v>
       </c>
       <c r="AF28" s="18">
         <v>2</v>
@@ -4894,7 +4929,8 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <v>113</v>
+        <f t="shared" ref="A29:A32" si="4">A28+1</f>
+        <v>23</v>
       </c>
       <c r="B29" s="10">
         <v>1</v>
@@ -4961,23 +4997,23 @@
       </c>
       <c r="X29" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="Y29" s="44">
         <f>Table5[[#This Row],[Result]]</f>
         <v>1</v>
       </c>
       <c r="Z29" s="45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AA29" s="45">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AA29" s="45">
-        <f>V47</f>
-        <v>1</v>
-      </c>
       <c r="AB29" s="45">
-        <f>V56</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="AC29" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
@@ -4988,8 +5024,8 @@
         <v>0</v>
       </c>
       <c r="AE29" s="59">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AF29" s="15">
         <v>1</v>
@@ -4997,7 +5033,8 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
-        <v>114</v>
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="B30" s="10">
         <v>4</v>
@@ -5064,23 +5101,23 @@
       </c>
       <c r="X30" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="Y30" s="44">
         <f>Table5[[#This Row],[Result]]</f>
         <v>5</v>
       </c>
       <c r="Z30" s="45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AA30" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AA30" s="45">
-        <f>V48</f>
-        <v>5</v>
-      </c>
       <c r="AB30" s="45">
-        <f>V57</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="AC30" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
@@ -5091,8 +5128,8 @@
         <v>0</v>
       </c>
       <c r="AE30" s="59">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
       <c r="AF30" s="15">
         <v>5</v>
@@ -5100,7 +5137,8 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
-        <v>115</v>
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
       <c r="B31" s="10">
         <v>5</v>
@@ -5169,23 +5207,23 @@
       </c>
       <c r="X31" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="Y31" s="44">
         <f>Table5[[#This Row],[Result]]</f>
         <v>4</v>
       </c>
       <c r="Z31" s="45">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AA31" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AA31" s="45">
-        <f>V49</f>
-        <v>4</v>
-      </c>
       <c r="AB31" s="45">
-        <f>V58</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="AC31" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
@@ -5196,15 +5234,18 @@
         <v>0</v>
       </c>
       <c r="AE31" s="59">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>14</v>
       </c>
       <c r="AF31" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="9">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -5258,7 +5299,7 @@
       <c r="V32" s="21"/>
       <c r="X32" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Y32" s="44">
         <f>Table5[[#This Row],[Result]]</f>
@@ -5269,12 +5310,12 @@
         <v>0</v>
       </c>
       <c r="AA32" s="45">
-        <f>V50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB32" s="45">
-        <f>V59</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="AC32" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
@@ -5285,8 +5326,8 @@
         <v>0</v>
       </c>
       <c r="AE32" s="59">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="AF32" s="18"/>
     </row>
@@ -5356,11 +5397,11 @@
         <v>0</v>
       </c>
       <c r="AA33" s="45">
-        <f>V51</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB33" s="45">
-        <f>V60</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC33" s="45">
@@ -5372,38 +5413,38 @@
         <v>0</v>
       </c>
       <c r="AE33" s="59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF33" s="15"/>
     </row>
     <row r="34" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="74" t="s">
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="88"/>
+      <c r="K34" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="75"/>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="75"/>
-      <c r="S34" s="75"/>
-      <c r="T34" s="75"/>
-      <c r="U34" s="75"/>
-      <c r="V34" s="76"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
+      <c r="U34" s="81"/>
+      <c r="V34" s="82"/>
       <c r="X34" s="48"/>
       <c r="Y34" s="49"/>
       <c r="Z34" s="49"/>
@@ -5486,8 +5527,8 @@
     </row>
     <row r="36" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <f t="shared" ref="A36:A42" si="2">A27</f>
-        <v>111</v>
+        <f t="shared" ref="A36:A42" si="5">A27</f>
+        <v>21</v>
       </c>
       <c r="B36" s="10">
         <v>3</v>
@@ -5546,14 +5587,14 @@
       </c>
       <c r="T36" s="55"/>
       <c r="U36" s="56"/>
-      <c r="V36" s="90">
+      <c r="V36" s="79">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
-        <f t="shared" si="2"/>
-        <v>112</v>
+        <f t="shared" si="5"/>
+        <v>22</v>
       </c>
       <c r="B37" s="10">
         <v>2</v>
@@ -5615,22 +5656,22 @@
       <c r="V37" s="27">
         <v>3</v>
       </c>
-      <c r="X37" s="85" t="s">
+      <c r="X37" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="Y37" s="86"/>
-      <c r="Z37" s="86"/>
-      <c r="AA37" s="86"/>
-      <c r="AB37" s="86"/>
-      <c r="AC37" s="86"/>
-      <c r="AD37" s="86"/>
-      <c r="AE37" s="86"/>
-      <c r="AF37" s="87"/>
+      <c r="Y37" s="77"/>
+      <c r="Z37" s="77"/>
+      <c r="AA37" s="77"/>
+      <c r="AB37" s="77"/>
+      <c r="AC37" s="77"/>
+      <c r="AD37" s="77"/>
+      <c r="AE37" s="77"/>
+      <c r="AF37" s="78"/>
     </row>
     <row r="38" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <f t="shared" si="2"/>
-        <v>113</v>
+        <f t="shared" si="5"/>
+        <v>23</v>
       </c>
       <c r="B38" s="10">
         <v>1</v>
@@ -5692,13 +5733,13 @@
       <c r="V38" s="27">
         <v>1</v>
       </c>
-      <c r="X38" s="80" t="s">
+      <c r="X38" s="71" t="s">
         <v>35</v>
       </c>
       <c r="Y38" s="69"/>
       <c r="Z38" s="69"/>
       <c r="AA38" s="69"/>
-      <c r="AB38" s="81"/>
+      <c r="AB38" s="72"/>
       <c r="AC38" s="68" t="s">
         <v>36</v>
       </c>
@@ -5708,8 +5749,8 @@
     </row>
     <row r="39" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <f t="shared" si="2"/>
-        <v>114</v>
+        <f t="shared" si="5"/>
+        <v>24</v>
       </c>
       <c r="B39" s="10">
         <v>5</v>
@@ -5801,8 +5842,8 @@
     </row>
     <row r="40" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
-        <f t="shared" si="2"/>
-        <v>115</v>
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="B40" s="10">
         <v>4</v>
@@ -5868,32 +5909,32 @@
         <v>111</v>
       </c>
       <c r="Y40" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f t="shared" ref="Y40:AE40" si="6">SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z40" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AA40" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AB40" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AC40" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AD40" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AE40" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AF40" s="8">
         <v>5</v>
@@ -5901,8 +5942,8 @@
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -5956,32 +5997,32 @@
         <v>112</v>
       </c>
       <c r="Y41" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$41)</f>
+        <f t="shared" ref="Y41:AE41" si="7">SUMIFS(K:K,$A:$A,$X$41)</f>
         <v>0</v>
       </c>
       <c r="Z41" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$41)</f>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AA41" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$41)</f>
-        <v>12</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AB41" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$41)</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AC41" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$41)</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AD41" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$41)</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AE41" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$41)</f>
-        <v>15</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AF41" s="11">
         <v>4</v>
@@ -5989,7 +6030,7 @@
     </row>
     <row r="42" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="B42" s="13"/>
@@ -6042,90 +6083,90 @@
       <c r="V42" s="37"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f t="shared" ref="Y42:AE45" si="8">SUMIFS(K:K,$A:$A,$X$40)</f>
         <v>0</v>
       </c>
       <c r="Z42" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AA42" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AB42" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AC42" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AD42" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AE42" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AF42" s="11"/>
     </row>
     <row r="43" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="78"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="74" t="s">
+      <c r="B43" s="87"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="87"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="88"/>
+      <c r="K43" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="75"/>
-      <c r="M43" s="75"/>
-      <c r="N43" s="75"/>
-      <c r="O43" s="75"/>
-      <c r="P43" s="75"/>
-      <c r="Q43" s="75"/>
-      <c r="R43" s="75"/>
-      <c r="S43" s="75"/>
-      <c r="T43" s="75"/>
-      <c r="U43" s="75"/>
-      <c r="V43" s="76"/>
+      <c r="L43" s="81"/>
+      <c r="M43" s="81"/>
+      <c r="N43" s="81"/>
+      <c r="O43" s="81"/>
+      <c r="P43" s="81"/>
+      <c r="Q43" s="81"/>
+      <c r="R43" s="81"/>
+      <c r="S43" s="81"/>
+      <c r="T43" s="81"/>
+      <c r="U43" s="81"/>
+      <c r="V43" s="82"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z43" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AA43" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AB43" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AC43" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AD43" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AE43" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AF43" s="11"/>
     </row>
@@ -6198,39 +6239,39 @@
       </c>
       <c r="X44" s="9"/>
       <c r="Y44" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z44" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AA44" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AB44" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AC44" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AD44" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AE44" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AF44" s="11"/>
     </row>
     <row r="45" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <f t="shared" ref="A45:A51" si="3">A27</f>
-        <v>111</v>
+        <f t="shared" ref="A45:A51" si="9">A27</f>
+        <v>21</v>
       </c>
       <c r="B45" s="10">
         <v>2</v>
@@ -6294,39 +6335,39 @@
       </c>
       <c r="X45" s="9"/>
       <c r="Y45" s="10">
-        <f>SUMIFS(K:K,$A:$A,$X$40)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z45" s="10">
-        <f>SUMIFS(L:L,$A:$A,$X$40)</f>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AA45" s="10">
-        <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AB45" s="10">
-        <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AC45" s="10">
-        <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AD45" s="10">
-        <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AE45" s="10">
-        <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AF45" s="11"/>
     </row>
     <row r="46" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
-        <f t="shared" si="3"/>
-        <v>112</v>
+        <f t="shared" si="9"/>
+        <v>22</v>
       </c>
       <c r="B46" s="10">
         <v>3</v>
@@ -6400,8 +6441,8 @@
     </row>
     <row r="47" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
-        <f t="shared" si="3"/>
-        <v>113</v>
+        <f t="shared" si="9"/>
+        <v>23</v>
       </c>
       <c r="B47" s="10">
         <v>1</v>
@@ -6466,8 +6507,8 @@
     </row>
     <row r="48" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
-        <f t="shared" si="3"/>
-        <v>114</v>
+        <f t="shared" si="9"/>
+        <v>24</v>
       </c>
       <c r="B48" s="10">
         <v>5</v>
@@ -6529,22 +6570,22 @@
       <c r="V48" s="27">
         <v>5</v>
       </c>
-      <c r="X48" s="85" t="s">
+      <c r="X48" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="Y48" s="86"/>
-      <c r="Z48" s="86"/>
-      <c r="AA48" s="86"/>
-      <c r="AB48" s="86"/>
-      <c r="AC48" s="86"/>
-      <c r="AD48" s="86"/>
-      <c r="AE48" s="86"/>
-      <c r="AF48" s="87"/>
+      <c r="Y48" s="77"/>
+      <c r="Z48" s="77"/>
+      <c r="AA48" s="77"/>
+      <c r="AB48" s="77"/>
+      <c r="AC48" s="77"/>
+      <c r="AD48" s="77"/>
+      <c r="AE48" s="77"/>
+      <c r="AF48" s="78"/>
     </row>
-    <row r="49" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
-        <f t="shared" si="3"/>
-        <v>115</v>
+        <f t="shared" si="9"/>
+        <v>25</v>
       </c>
       <c r="B49" s="10">
         <v>4</v>
@@ -6606,13 +6647,13 @@
       <c r="V49" s="35">
         <v>4</v>
       </c>
-      <c r="X49" s="80" t="s">
+      <c r="X49" s="71" t="s">
         <v>35</v>
       </c>
       <c r="Y49" s="69"/>
       <c r="Z49" s="69"/>
       <c r="AA49" s="69"/>
-      <c r="AB49" s="81"/>
+      <c r="AB49" s="72"/>
       <c r="AC49" s="68" t="s">
         <v>36</v>
       </c>
@@ -6620,10 +6661,10 @@
       <c r="AE49" s="69"/>
       <c r="AF49" s="70"/>
     </row>
-    <row r="50" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>26</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -6701,9 +6742,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B51" s="13"/>
@@ -6767,55 +6808,55 @@
       </c>
       <c r="AA51" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AB51" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AD51" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AE51" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AF51" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="71" t="s">
+    <row r="52" spans="1:34" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="73"/>
-      <c r="K52" s="74" t="s">
+      <c r="B52" s="90"/>
+      <c r="C52" s="90"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="90"/>
+      <c r="J52" s="91"/>
+      <c r="K52" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="L52" s="75"/>
-      <c r="M52" s="75"/>
-      <c r="N52" s="75"/>
-      <c r="O52" s="75"/>
-      <c r="P52" s="75"/>
-      <c r="Q52" s="75"/>
-      <c r="R52" s="75"/>
-      <c r="S52" s="75"/>
-      <c r="T52" s="75"/>
-      <c r="U52" s="75"/>
-      <c r="V52" s="76"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="81"/>
+      <c r="Q52" s="81"/>
+      <c r="R52" s="81"/>
+      <c r="S52" s="81"/>
+      <c r="T52" s="81"/>
+      <c r="U52" s="81"/>
+      <c r="V52" s="82"/>
       <c r="X52" s="5" t="s">
         <v>70</v>
       </c>
@@ -6829,29 +6870,29 @@
       </c>
       <c r="AA52" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$41)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AB52" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$41)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AC52" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$41)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AD52" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$41)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AE52" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$41)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AF52" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>0</v>
       </c>
@@ -6879,494 +6920,656 @@
       <c r="I53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="38" t="s">
+      <c r="L53" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M53" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="L53" s="34" t="s">
+      <c r="N53" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="34" t="s">
+      <c r="O53" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N53" s="34" t="s">
+      <c r="P53" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O53" s="34" t="s">
+      <c r="Q53" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="P53" s="34" t="s">
+      <c r="R53" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q53" s="34" t="s">
+      <c r="S53" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R53" s="41" t="s">
+      <c r="T53" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="S53" s="17" t="s">
+      <c r="U53" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="T53" s="17" t="s">
+      <c r="V53" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="U53" s="17" t="s">
+      <c r="W53" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="V53" s="39" t="s">
+      <c r="X53" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="X53" s="5" t="s">
+      <c r="Z53" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="Y53" s="10">
+      <c r="AA53" s="10">
         <f>SUMIF(B45:F45, "&lt;=3")</f>
         <v>7</v>
       </c>
-      <c r="Z53" s="10">
+      <c r="AB53" s="10">
         <f>SUMIF(B46:F46, "&lt;=3")</f>
         <v>12</v>
       </c>
-      <c r="AA53" s="10">
+      <c r="AC53" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
-      </c>
-      <c r="AB53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AC53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AD53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AE53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AF53" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH53" s="11"/>
     </row>
-    <row r="54" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <f t="shared" ref="A54:A60" si="4">A27</f>
-        <v>111</v>
-      </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="19">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q54" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R54" s="20">
+        <f t="shared" ref="A54:A60" si="10">A27</f>
+        <v>21</v>
+      </c>
+      <c r="B54" s="10">
+        <v>2</v>
+      </c>
+      <c r="C54" s="10">
+        <v>4</v>
+      </c>
+      <c r="D54" s="10">
+        <v>6</v>
+      </c>
+      <c r="E54" s="10">
+        <v>6</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1</v>
+      </c>
+      <c r="G54" s="6">
+        <v>3</v>
+      </c>
+      <c r="H54" s="7">
+        <v>2</v>
+      </c>
+      <c r="I54" s="7">
+        <v>3</v>
+      </c>
+      <c r="J54" s="7">
+        <v>5</v>
+      </c>
+      <c r="K54" s="7">
+        <v>5</v>
+      </c>
+      <c r="L54" s="8">
+        <v>5</v>
+      </c>
+      <c r="M54" s="54">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>1</v>
+      </c>
+      <c r="N54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>3</v>
+      </c>
+      <c r="O54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>5</v>
+      </c>
+      <c r="P54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>6</v>
+      </c>
+      <c r="Q54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>9</v>
+      </c>
+      <c r="R54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S54" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T54" s="55">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S54" s="55">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T54" s="20"/>
-      <c r="U54" s="31"/>
-      <c r="V54" s="27"/>
-      <c r="X54" s="5"/>
-      <c r="Y54" s="10"/>
-      <c r="Z54" s="10"/>
-      <c r="AA54" s="10">
+        <v>5</v>
+      </c>
+      <c r="U54" s="55">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>11</v>
+      </c>
+      <c r="V54" s="55"/>
+      <c r="W54" s="56"/>
+      <c r="X54" s="27">
+        <v>6</v>
+      </c>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="10"/>
+      <c r="AB54" s="10"/>
+      <c r="AC54" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
-      </c>
-      <c r="AB54" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AC54" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE54" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AD54" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF54" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AE54" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG54" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AF54" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH54" s="11"/>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
-        <f t="shared" si="4"/>
-        <v>112</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="26">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q55" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R55" s="20">
+        <f t="shared" si="10"/>
+        <v>22</v>
+      </c>
+      <c r="B55" s="10">
+        <v>4</v>
+      </c>
+      <c r="C55" s="10">
+        <v>1</v>
+      </c>
+      <c r="D55" s="10">
+        <v>5</v>
+      </c>
+      <c r="E55" s="10">
+        <v>1</v>
+      </c>
+      <c r="F55" s="10">
+        <v>2</v>
+      </c>
+      <c r="G55" s="10">
+        <v>4</v>
+      </c>
+      <c r="H55" s="10">
+        <v>3</v>
+      </c>
+      <c r="I55" s="10">
+        <v>5</v>
+      </c>
+      <c r="J55" s="10">
+        <v>1</v>
+      </c>
+      <c r="K55" s="10">
+        <v>1</v>
+      </c>
+      <c r="L55" s="11">
+        <v>4</v>
+      </c>
+      <c r="M55" s="92">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>4</v>
+      </c>
+      <c r="N55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>5</v>
+      </c>
+      <c r="O55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>6</v>
+      </c>
+      <c r="P55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>9</v>
+      </c>
+      <c r="Q55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>11</v>
+      </c>
+      <c r="R55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S55" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T55" s="55">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S55" s="20">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T55" s="20"/>
-      <c r="U55" s="31"/>
-      <c r="V55" s="27"/>
-      <c r="X55" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="U55" s="55">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>9</v>
+      </c>
+      <c r="V55" s="55"/>
+      <c r="W55" s="56"/>
+      <c r="X55" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Y55" s="10">
+      <c r="AA55" s="10">
         <f>SUM(Y51:Y53)</f>
-        <v>30</v>
-      </c>
-      <c r="Z55" s="10">
+        <v>23</v>
+      </c>
+      <c r="AB55" s="10">
         <f>SUM(Z51:Z53)</f>
-        <v>29</v>
-      </c>
-      <c r="AA55" s="10">
+        <v>17</v>
+      </c>
+      <c r="AC55" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
-      </c>
-      <c r="AB55" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD55" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AC55" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE55" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AD55" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF55" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AE55" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG55" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AF55" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH55" s="11"/>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
-        <f t="shared" si="4"/>
-        <v>113</v>
-      </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="26">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q56" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R56" s="20">
+        <f t="shared" si="10"/>
+        <v>23</v>
+      </c>
+      <c r="B56" s="10">
+        <v>3</v>
+      </c>
+      <c r="C56" s="10">
+        <v>3</v>
+      </c>
+      <c r="D56" s="10">
+        <v>4</v>
+      </c>
+      <c r="E56" s="10">
+        <v>4</v>
+      </c>
+      <c r="F56" s="10">
+        <v>4</v>
+      </c>
+      <c r="G56" s="10">
+        <v>6</v>
+      </c>
+      <c r="H56" s="10">
+        <v>5</v>
+      </c>
+      <c r="I56" s="10">
+        <v>5</v>
+      </c>
+      <c r="J56" s="10">
+        <v>2</v>
+      </c>
+      <c r="K56" s="10">
+        <v>3</v>
+      </c>
+      <c r="L56" s="11">
+        <v>6</v>
+      </c>
+      <c r="M56" s="92">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="N56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>1</v>
+      </c>
+      <c r="O56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>4</v>
+      </c>
+      <c r="P56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>7</v>
+      </c>
+      <c r="Q56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>9</v>
+      </c>
+      <c r="R56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S56" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T56" s="55">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S56" s="20">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T56" s="20"/>
-      <c r="U56" s="31"/>
-      <c r="V56" s="27"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="10"/>
-      <c r="Z56" s="10"/>
-      <c r="AA56" s="10">
+        <v>5</v>
+      </c>
+      <c r="U56" s="55">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>11</v>
+      </c>
+      <c r="V56" s="55"/>
+      <c r="W56" s="56"/>
+      <c r="X56" s="27">
+        <v>5</v>
+      </c>
+      <c r="Z56" s="9"/>
+      <c r="AA56" s="10"/>
+      <c r="AB56" s="10"/>
+      <c r="AC56" s="10">
         <f>SUMIFS(M:M,$A:$A,$X$40)</f>
-        <v>12</v>
-      </c>
-      <c r="AB56" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD56" s="10">
         <f>SUMIFS(N:N,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AC56" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE56" s="10">
         <f>SUMIFS(O:O,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AD56" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF56" s="10">
         <f>SUMIFS(P:P,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AE56" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG56" s="10">
         <f>SUMIFS(Q:Q,$A:$A,$X$40)</f>
-        <v>15</v>
-      </c>
-      <c r="AF56" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH56" s="11"/>
     </row>
-    <row r="57" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <f t="shared" si="4"/>
-        <v>114</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="26">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q57" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R57" s="20">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="B57" s="10">
+        <v>1</v>
+      </c>
+      <c r="C57" s="10">
+        <v>6</v>
+      </c>
+      <c r="D57" s="10">
+        <v>1</v>
+      </c>
+      <c r="E57" s="10">
+        <v>3</v>
+      </c>
+      <c r="F57" s="10">
+        <v>5</v>
+      </c>
+      <c r="G57" s="10">
+        <v>5</v>
+      </c>
+      <c r="H57" s="10">
+        <v>6</v>
+      </c>
+      <c r="I57" s="10">
+        <v>1</v>
+      </c>
+      <c r="J57" s="10">
+        <v>6</v>
+      </c>
+      <c r="K57" s="10">
+        <v>2</v>
+      </c>
+      <c r="L57" s="11">
+        <v>3</v>
+      </c>
+      <c r="M57" s="92">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>4</v>
+      </c>
+      <c r="O57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>6</v>
+      </c>
+      <c r="P57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>6</v>
+      </c>
+      <c r="Q57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>8</v>
+      </c>
+      <c r="R57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S57" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T57" s="55">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S57" s="20">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T57" s="20"/>
-      <c r="U57" s="31"/>
-      <c r="V57" s="27"/>
-      <c r="X57" s="12"/>
-      <c r="Y57" s="13"/>
-      <c r="Z57" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="U57" s="55">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>11</v>
+      </c>
+      <c r="V57" s="55"/>
+      <c r="W57" s="56"/>
+      <c r="X57" s="27">
+        <v>3</v>
+      </c>
+      <c r="Z57" s="12"/>
       <c r="AA57" s="13"/>
       <c r="AB57" s="13"/>
       <c r="AC57" s="13"/>
       <c r="AD57" s="13"/>
-      <c r="AE57" s="14"/>
-      <c r="AF57" s="14"/>
+      <c r="AE57" s="13"/>
+      <c r="AF57" s="13"/>
+      <c r="AG57" s="14"/>
+      <c r="AH57" s="14"/>
     </row>
-    <row r="58" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
-        <f t="shared" si="4"/>
-        <v>115</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="28">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q58" s="22">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R58" s="22">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="B58" s="10">
+        <v>5</v>
+      </c>
+      <c r="C58" s="10">
+        <v>5</v>
+      </c>
+      <c r="D58" s="10">
+        <v>3</v>
+      </c>
+      <c r="E58" s="10">
+        <v>2</v>
+      </c>
+      <c r="F58" s="10">
+        <v>6</v>
+      </c>
+      <c r="G58" s="10">
+        <v>1</v>
+      </c>
+      <c r="H58" s="10">
+        <v>1</v>
+      </c>
+      <c r="I58" s="10">
+        <v>2</v>
+      </c>
+      <c r="J58" s="10">
+        <v>4</v>
+      </c>
+      <c r="K58" s="10">
+        <v>4</v>
+      </c>
+      <c r="L58" s="11">
+        <v>1</v>
+      </c>
+      <c r="M58" s="93">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>3</v>
+      </c>
+      <c r="N58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>5</v>
+      </c>
+      <c r="O58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>6</v>
+      </c>
+      <c r="P58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>8</v>
+      </c>
+      <c r="Q58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>10</v>
+      </c>
+      <c r="R58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S58" s="65">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T58" s="65">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S58" s="22">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T58" s="22"/>
-      <c r="U58" s="32"/>
-      <c r="V58" s="35"/>
+        <v>5</v>
+      </c>
+      <c r="U58" s="65">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>10</v>
+      </c>
+      <c r="V58" s="65"/>
+      <c r="W58" s="66"/>
+      <c r="X58" s="35">
+        <v>2</v>
+      </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="26">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
-      </c>
-      <c r="N59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q59" s="20">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
-      </c>
-      <c r="R59" s="20">
+        <f t="shared" si="10"/>
+        <v>26</v>
+      </c>
+      <c r="B59" s="10">
+        <v>6</v>
+      </c>
+      <c r="C59" s="10">
+        <v>2</v>
+      </c>
+      <c r="D59" s="10">
+        <v>2</v>
+      </c>
+      <c r="E59" s="10">
+        <v>5</v>
+      </c>
+      <c r="F59" s="10">
+        <v>3</v>
+      </c>
+      <c r="G59" s="10">
+        <v>2</v>
+      </c>
+      <c r="H59" s="10">
+        <v>4</v>
+      </c>
+      <c r="I59" s="10">
+        <v>6</v>
+      </c>
+      <c r="J59" s="10">
+        <v>3</v>
+      </c>
+      <c r="K59" s="10">
+        <v>6</v>
+      </c>
+      <c r="L59" s="11">
+        <v>2</v>
+      </c>
+      <c r="M59" s="92">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="N59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
+        <v>4</v>
+      </c>
+      <c r="O59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>6</v>
+      </c>
+      <c r="P59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
+        <v>7</v>
+      </c>
+      <c r="Q59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
+        <v>8</v>
+      </c>
+      <c r="R59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>11</v>
+      </c>
+      <c r="S59" s="55">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>11</v>
+      </c>
+      <c r="T59" s="55">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
-      </c>
-      <c r="S59" s="20">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T59" s="20"/>
-      <c r="U59" s="31"/>
-      <c r="V59" s="27"/>
+        <v>5</v>
+      </c>
+      <c r="U59" s="55">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>14</v>
+      </c>
+      <c r="V59" s="55"/>
+      <c r="W59" s="56"/>
+      <c r="X59" s="27">
+        <v>4</v>
+      </c>
     </row>
-    <row r="60" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="B60" s="13"/>
@@ -7377,49 +7580,51 @@
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="29">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="29">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]], 1)</f>
         <v>0</v>
       </c>
       <c r="N60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=2")</f>
         <v>0</v>
       </c>
       <c r="O60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
         <v>0</v>
       </c>
       <c r="P60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=4")</f>
         <v>0</v>
       </c>
       <c r="Q60" s="30">
-        <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=5")</f>
         <v>0</v>
       </c>
       <c r="R60" s="30">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=6")</f>
+        <v>0</v>
+      </c>
+      <c r="S60" s="30">
+        <f>COUNTIF(Table8[[#This Row],[A]:[K]],"&lt;=7")</f>
+        <v>0</v>
+      </c>
+      <c r="T60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S60" s="30">
-        <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T60" s="30"/>
-      <c r="U60" s="36"/>
-      <c r="V60" s="37"/>
+      <c r="U60" s="30">
+        <f>SUMIF(Table8[[#This Row],[A]:[K]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="30"/>
+      <c r="W60" s="36"/>
+      <c r="X60" s="37"/>
     </row>
-    <row r="61" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>41</v>
       </c>
@@ -7430,7 +7635,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>42</v>
       </c>
@@ -7441,7 +7646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>43</v>
       </c>
@@ -7452,7 +7657,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>44</v>
       </c>
@@ -7463,7 +7668,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>45</v>
       </c>
@@ -7474,7 +7679,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>46</v>
       </c>
@@ -7482,86 +7687,100 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
       <c r="F70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>65</v>
       </c>
       <c r="G72" t="s">
         <v>74</v>
       </c>
+      <c r="K72" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>58</v>
       </c>
       <c r="G73" t="s">
         <v>75</v>
       </c>
+      <c r="K73" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>59</v>
       </c>
       <c r="G74" t="s">
         <v>76</v>
       </c>
+      <c r="K74" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>60</v>
       </c>
       <c r="G75" t="s">
         <v>77</v>
       </c>
+      <c r="K75" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>61</v>
       </c>
       <c r="G76" t="s">
         <v>78</v>
       </c>
+      <c r="K76" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>62</v>
       </c>
       <c r="G77" t="s">
         <v>79</v>
       </c>
+      <c r="K77" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>63</v>
       </c>
+      <c r="K78" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="K25:V25"/>
-    <mergeCell ref="X25:AF25"/>
-    <mergeCell ref="X37:AF37"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="K34:V34"/>
-    <mergeCell ref="AC38:AF38"/>
+  <mergeCells count="8">
     <mergeCell ref="A52:J52"/>
     <mergeCell ref="K52:V52"/>
     <mergeCell ref="K43:V43"/>
     <mergeCell ref="A43:J43"/>
-    <mergeCell ref="X38:AB38"/>
-    <mergeCell ref="X48:AF48"/>
-    <mergeCell ref="X49:AB49"/>
-    <mergeCell ref="AC49:AF49"/>
+    <mergeCell ref="K25:V25"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="K34:V34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>